<commit_message>
Inserted a figure in latex, and turned exclude_lenless2 off
</commit_message>
<xml_diff>
--- a/write-ups/cikm/performance.xlsx
+++ b/write-ups/cikm/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15780" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change with Epochlength" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="121">
   <si>
     <t>MinSupp</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Ngram Len</t>
   </si>
   <si>
-    <t>Avg Itemsets</t>
-  </si>
-  <si>
     <t>Stdev</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
   </si>
   <si>
     <t>Upper CI band</t>
-  </si>
-  <si>
-    <t>Avg Distinct Terms</t>
   </si>
   <si>
     <t>Avg. Distinct Terms</t>
@@ -354,12 +348,54 @@
   <si>
     <t>Overconf</t>
   </si>
+  <si>
+    <t>TweetsSkipped</t>
+  </si>
+  <si>
+    <t>TweetsNet</t>
+  </si>
+  <si>
+    <t>ItemsetsCount</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>TweetsVolume</t>
+  </si>
+  <si>
+    <t>WallMillisMining</t>
+  </si>
+  <si>
+    <t>[1349085600, 1357038000, file:///home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec, 3600/1800, /home/yaboulna/fimi/lcm53/lcm CfI, &gt;10, 5]</t>
+  </si>
+  <si>
+    <t>[1351764000, 1354273200, file:///home/yaboulna/fim_out/lcm_closed_cikm/bg_1hr+1hr_ngram1-relsupp10_nov, 3600/3600, /home/yaboulna/fimi/lcm53/lcm Cf, &gt;10, 1]</t>
+  </si>
+  <si>
+    <t>[1351764000, 1354273200, file:///home/yaboulna/fim_out/lcm_closed_cikm/bg_1hr+1hr_ngram4-relsupp10_nov, 3600/3600, /home/yaboulna/fimi/lcm53/lcm Cf, &gt;10, 4]</t>
+  </si>
+  <si>
+    <t>[1351764000, 1354273200, file:///home/yaboulna/fim_out/lcm_closed_cikm/bg_1hr+1hr_ngram2-relsupp10_nov, 3600/3600, /home/yaboulna/fimi/lcm53/lcm Cf, &gt;10, 2]</t>
+  </si>
+  <si>
+    <t>[1351764000, 1354273200, file:///home/yaboulna/fim_out/lcm_closed_cikm/bg_1hr+1hr_ngram3-relsupp10_nov, 3600/3600, /home/yaboulna/fimi/lcm53/lcm Cf, &gt;10, 3]</t>
+  </si>
+  <si>
+    <t>Runtime in Milliseconds</t>
+  </si>
+  <si>
+    <t>Mean number of iItemsets</t>
+  </si>
+  <si>
+    <t>Mean number of distinct terms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,6 +426,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -408,7 +450,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="205">
+  <cellStyleXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -614,13 +656,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="205">
+  <cellStyles count="221">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -723,6 +782,14 @@
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -825,6 +892,14 @@
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1055,10 +1130,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1074,7 +1146,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg Distinct Terms</c:v>
+                  <c:v>Mean number of distinct terms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1087,19 +1159,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>185906.047345768</c:v>
+                  <c:v>185906.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>557687.00143472</c:v>
+                  <c:v>557687.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>589020.37302726</c:v>
+                  <c:v>589020.37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>589129.137733142</c:v>
+                  <c:v>589129.14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>569848.162516976</c:v>
+                  <c:v>569848.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1151,8 +1223,281 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Change with ngram len'!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean number of distinct terms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Change with ngram len'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Change with ngram len'!$N$2:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>185.906</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>557.687</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>589.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>589.129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>569.848</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Change with ngram len'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean number of iItemsets</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Change with ngram len'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Change with ngram len'!$J$2:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>61505.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6981.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6292.86</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>6260.393113342898</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>6146.53856975381</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Change with ngram len'!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Runtime in Milliseconds</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Change with ngram len'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Change with ngram len'!$R$2:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1302.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>607.49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>577.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>445.51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>489.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2126493992"/>
+        <c:axId val="-2126490904"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2126493992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2126490904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2126490904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2126493992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1167,7 +1512,151 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Change with ngram len'!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Runtime in Milliseconds</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Change with ngram len'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Change with ngram len'!$R$2:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1302.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>607.49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>577.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>445.51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>489.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-25"/>
+        <c:axId val="-2113928040"/>
+        <c:axId val="-2113062056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2113928040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2113062056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2113062056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2113928040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1440,7 +1929,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1761,7 +2250,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1930,7 +2419,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2061,7 +2550,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2181,7 +2670,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2301,7 +2790,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2446,7 +2935,146 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Change with Epochlength'!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Distinct Terms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Change with Epochlength'!$P$2:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>71970.5784444999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>181224.929266636</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>569848.162516976</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.08354324231465E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.49974681081081E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.36463622666667E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.49602949E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2130089992"/>
+        <c:axId val="-2130086984"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2130089992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2130086984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2130086984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2130089992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2591,7 +3219,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2782,144 +3410,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Change with Epochlength'!$P$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Avg. Distinct Terms</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Change with Epochlength'!$P$2:$P$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>71970.5784444999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>181224.929266636</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>569848.162516976</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.08354324231465E6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.49974681081081E6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.36463622666667E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.49602949E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2130089992"/>
-        <c:axId val="-2130086984"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-2130089992"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130086984"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2130086984"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130089992"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-      </c:dTable>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3215,6 +3706,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3271,6 +3763,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3365,6 +3858,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3428,6 +3922,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3583,6 +4078,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3762,6 +4258,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4421,30 +4918,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Avg Number of Itemsets in an hour, at different N-Gram</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> lengthes</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -4460,7 +4934,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg Itemsets</c:v>
+                  <c:v>Mean number of iItemsets</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4473,18 +4947,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>61505.1549497848</c:v>
+                  <c:v>61505.16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6981.75620437956</c:v>
+                  <c:v>6981.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6292.85078909613</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                  <c:v>6292.86</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
                   <c:v>6260.393113342898</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="4" formatCode="0.00">
                   <c:v>6146.53856975381</c:v>
                 </c:pt>
               </c:numCache>
@@ -4537,10 +5011,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4802,16 +5272,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25401</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>450400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>148998</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4833,15 +5303,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:colOff>25401</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>145600</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>72800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4855,6 +5325,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>136300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5507,7 +6037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S95"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
@@ -5527,7 +6057,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -5536,13 +6066,13 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -5563,7 +6093,7 @@
         <v>5</v>
       </c>
       <c r="P1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -5571,7 +6101,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>1512.0237</v>
@@ -5625,7 +6155,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>6409.9687999999996</v>
@@ -5679,7 +6209,7 @@
     </row>
     <row r="4" spans="1:19">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>1762.973</v>
@@ -5733,7 +6263,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>1552.1977999999999</v>
@@ -5787,7 +6317,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>1426.5217</v>
@@ -5841,7 +6371,7 @@
     </row>
     <row r="7" spans="1:19">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>3242.7777999999998</v>
@@ -5895,7 +6425,7 @@
     </row>
     <row r="8" spans="1:19">
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>635074.79021450004</v>
@@ -5946,7 +6476,7 @@
     </row>
     <row r="32" spans="5:5">
       <c r="E32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:12">
@@ -5964,7 +6494,7 @@
         <v>1662.2942</v>
       </c>
       <c r="I33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="2:12">
@@ -6254,12 +6784,12 @@
     </row>
     <row r="65" spans="2:7">
       <c r="D65" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="2:7">
       <c r="B66" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C66">
         <v>3805</v>
@@ -6279,7 +6809,7 @@
     </row>
     <row r="67" spans="2:7">
       <c r="B67" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C67">
         <v>1282</v>
@@ -6299,7 +6829,7 @@
     </row>
     <row r="68" spans="2:7">
       <c r="B68" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C68">
         <v>4265</v>
@@ -6319,7 +6849,7 @@
     </row>
     <row r="69" spans="2:7">
       <c r="B69" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C69">
         <v>364</v>
@@ -6339,7 +6869,7 @@
     </row>
     <row r="70" spans="2:7">
       <c r="B70" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C70">
         <v>184</v>
@@ -6359,7 +6889,7 @@
     </row>
     <row r="71" spans="2:7">
       <c r="B71" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C71">
         <v>18</v>
@@ -6379,21 +6909,21 @@
     </row>
     <row r="89" spans="5:9">
       <c r="F89" t="s">
+        <v>86</v>
+      </c>
+      <c r="G89" t="s">
+        <v>85</v>
+      </c>
+      <c r="H89" t="s">
+        <v>87</v>
+      </c>
+      <c r="I89" t="s">
         <v>88</v>
-      </c>
-      <c r="G89" t="s">
-        <v>87</v>
-      </c>
-      <c r="H89" t="s">
-        <v>89</v>
-      </c>
-      <c r="I89" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="90" spans="5:9">
       <c r="E90" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F90">
         <v>6409.9687999999996</v>
@@ -6411,7 +6941,7 @@
     </row>
     <row r="91" spans="5:9">
       <c r="E91" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F91">
         <v>1762.973</v>
@@ -6429,7 +6959,7 @@
     </row>
     <row r="92" spans="5:9">
       <c r="E92" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F92">
         <v>1552.1977999999999</v>
@@ -6447,12 +6977,12 @@
     </row>
     <row r="93" spans="5:9">
       <c r="E93" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="5:9">
       <c r="E94" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F94">
         <v>1426.5217</v>
@@ -6470,7 +7000,7 @@
     </row>
     <row r="95" spans="5:9">
       <c r="E95" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F95">
         <v>3242.7777999999998</v>
@@ -6500,20 +7030,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -6524,16 +7055,16 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
@@ -6542,19 +7073,25 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>3600</v>
       </c>
@@ -6565,7 +7102,7 @@
         <v>697</v>
       </c>
       <c r="D2">
-        <v>185906.04734576799</v>
+        <v>185906.04</v>
       </c>
       <c r="E2">
         <v>30212.533124056099</v>
@@ -6583,7 +7120,7 @@
         <v>697</v>
       </c>
       <c r="J2">
-        <v>61505.154949784803</v>
+        <v>61505.16</v>
       </c>
       <c r="K2">
         <v>13106.913402203199</v>
@@ -6594,8 +7131,29 @@
       <c r="M2">
         <v>61542.012267242899</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>185.90600000000001</v>
+      </c>
+      <c r="O2" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q2">
+        <v>697</v>
+      </c>
+      <c r="R2">
+        <v>1302.0999999999999</v>
+      </c>
+      <c r="S2">
+        <v>1085.8462686391899</v>
+      </c>
+      <c r="T2">
+        <v>3.0534557912952698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -6606,7 +7164,7 @@
         <v>697</v>
       </c>
       <c r="D3">
-        <v>557687.00143472</v>
+        <v>557687</v>
       </c>
       <c r="E3">
         <v>100593.445636848</v>
@@ -6624,7 +7182,7 @@
         <v>685</v>
       </c>
       <c r="J3">
-        <v>6981.7562043795597</v>
+        <v>6981.76</v>
       </c>
       <c r="K3">
         <v>585.172302168633</v>
@@ -6635,8 +7193,29 @@
       <c r="M3">
         <v>6983.4305660032896</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>557.68700000000001</v>
+      </c>
+      <c r="O3" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q3">
+        <v>697</v>
+      </c>
+      <c r="R3">
+        <v>607.49</v>
+      </c>
+      <c r="S3">
+        <v>1363.9542754398201</v>
+      </c>
+      <c r="T3">
+        <v>3.8355098706772401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -6647,7 +7226,7 @@
         <v>697</v>
       </c>
       <c r="D4">
-        <v>589020.37302725995</v>
+        <v>589020.37</v>
       </c>
       <c r="E4">
         <v>108742.133485342</v>
@@ -6665,7 +7244,7 @@
         <v>697</v>
       </c>
       <c r="J4">
-        <v>6292.85078909613</v>
+        <v>6292.86</v>
       </c>
       <c r="K4">
         <v>340.25846852836298</v>
@@ -6676,8 +7255,29 @@
       <c r="M4">
         <v>6293.8076134839503</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4">
+        <v>589.02</v>
+      </c>
+      <c r="O4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P4" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q4">
+        <v>697</v>
+      </c>
+      <c r="R4">
+        <v>577.15</v>
+      </c>
+      <c r="S4">
+        <v>1276.43662844707</v>
+      </c>
+      <c r="T4">
+        <v>3.5894057270534501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="B5">
         <v>4</v>
       </c>
@@ -6685,7 +7285,7 @@
         <v>697</v>
       </c>
       <c r="D5">
-        <v>589129.13773314201</v>
+        <v>589129.14</v>
       </c>
       <c r="E5">
         <v>108818.468100659</v>
@@ -6702,15 +7302,36 @@
       <c r="I5">
         <v>697</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <f>K5/I5</f>
         <v>6260.3931133428978</v>
       </c>
       <c r="K5">
         <v>4363494</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>589.12900000000002</v>
+      </c>
+      <c r="O5" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q5">
+        <v>697</v>
+      </c>
+      <c r="R5">
+        <v>445.51</v>
+      </c>
+      <c r="S5">
+        <v>404.09486588419003</v>
+      </c>
+      <c r="T5">
+        <v>1.13633563433718</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="B6">
         <v>5</v>
       </c>
@@ -6718,7 +7339,7 @@
         <v>4418</v>
       </c>
       <c r="D6">
-        <v>569848.16251697601</v>
+        <v>569848.16</v>
       </c>
       <c r="E6">
         <v>151586.72571426499</v>
@@ -6735,7 +7356,8 @@
       <c r="I6">
         <v>4265</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
+        <f>6146.53856975381</f>
         <v>6146.5385697538104</v>
       </c>
       <c r="K6">
@@ -6747,8 +7369,790 @@
       <c r="M6">
         <v>6146.8739335056098</v>
       </c>
+      <c r="N6">
+        <v>569.84799999999996</v>
+      </c>
+      <c r="O6" t="s">
+        <v>113</v>
+      </c>
+      <c r="P6" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q6">
+        <v>4418</v>
+      </c>
+      <c r="R6">
+        <v>489.85</v>
+      </c>
+      <c r="S6">
+        <v>786.935533612276</v>
+      </c>
+      <c r="T6">
+        <v>0.34911580938887699</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34">
+        <v>4418</v>
+      </c>
+      <c r="E34">
+        <v>569848.16</v>
+      </c>
+      <c r="F34">
+        <v>151586.72571426499</v>
+      </c>
+      <c r="G34">
+        <v>67.249882842906203</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35">
+        <v>697</v>
+      </c>
+      <c r="E35">
+        <v>185906.05</v>
+      </c>
+      <c r="F35">
+        <v>30212.533124056099</v>
+      </c>
+      <c r="G35">
+        <v>84.959203620014193</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36">
+        <v>697</v>
+      </c>
+      <c r="E36">
+        <v>589129.14</v>
+      </c>
+      <c r="F36">
+        <v>108818.468100659</v>
+      </c>
+      <c r="G36">
+        <v>306.00315276512401</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37">
+        <v>697</v>
+      </c>
+      <c r="E37">
+        <v>557687</v>
+      </c>
+      <c r="F37">
+        <v>100593.445636848</v>
+      </c>
+      <c r="G37">
+        <v>282.87396477506599</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38">
+        <v>697</v>
+      </c>
+      <c r="E38">
+        <v>589020.37</v>
+      </c>
+      <c r="F38">
+        <v>108742.133485342</v>
+      </c>
+      <c r="G38">
+        <v>305.78849588417597</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39">
+        <v>697</v>
+      </c>
+      <c r="E39">
+        <v>6983.3</v>
+      </c>
+      <c r="F39">
+        <v>583.70063960778702</v>
+      </c>
+      <c r="G39">
+        <v>1.64139634667326</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40">
+        <v>697</v>
+      </c>
+      <c r="E40">
+        <v>61505.15</v>
+      </c>
+      <c r="F40">
+        <v>13106.913402203199</v>
+      </c>
+      <c r="G40">
+        <v>36.8573174581323</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41">
+        <v>697</v>
+      </c>
+      <c r="E41">
+        <v>6292.85</v>
+      </c>
+      <c r="F41">
+        <v>340.25846852836298</v>
+      </c>
+      <c r="G41">
+        <v>0.95682438782724799</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>697</v>
+      </c>
+      <c r="E42">
+        <v>20.12</v>
+      </c>
+      <c r="F42">
+        <v>4.8995866296700497</v>
+      </c>
+      <c r="G42">
+        <v>1.37778906659301E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>697</v>
+      </c>
+      <c r="E43">
+        <v>20.12</v>
+      </c>
+      <c r="F43">
+        <v>4.8995866296700497</v>
+      </c>
+      <c r="G43">
+        <v>1.37778906659301E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>697</v>
+      </c>
+      <c r="E44">
+        <v>20.12</v>
+      </c>
+      <c r="F44">
+        <v>4.8995866296700497</v>
+      </c>
+      <c r="G44">
+        <v>1.37778906659301E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>4418</v>
+      </c>
+      <c r="E45">
+        <v>19.53</v>
+      </c>
+      <c r="F45">
+        <v>5.6611586883426996</v>
+      </c>
+      <c r="G45">
+        <v>2.51151449279124E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>697</v>
+      </c>
+      <c r="E46">
+        <v>20.12</v>
+      </c>
+      <c r="F46">
+        <v>4.8995866296700497</v>
+      </c>
+      <c r="G46">
+        <v>1.37778906659301E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47">
+        <v>697</v>
+      </c>
+      <c r="E47">
+        <v>1366704953008.8</v>
+      </c>
+      <c r="F47">
+        <v>6082969.0713838898</v>
+      </c>
+      <c r="G47">
+        <v>17105.623213647701</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48">
+        <v>4418</v>
+      </c>
+      <c r="E48">
+        <v>1366559785186.4099</v>
+      </c>
+      <c r="F48">
+        <v>23983788.1295821</v>
+      </c>
+      <c r="G48">
+        <v>10640.1595142555</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49">
+        <v>697</v>
+      </c>
+      <c r="E49">
+        <v>1366704611784.75</v>
+      </c>
+      <c r="F49">
+        <v>5833052.2664556503</v>
+      </c>
+      <c r="G49">
+        <v>16402.8442500044</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50">
+        <v>697</v>
+      </c>
+      <c r="E50">
+        <v>1366705834825.1101</v>
+      </c>
+      <c r="F50">
+        <v>6490827.9266444296</v>
+      </c>
+      <c r="G50">
+        <v>18252.5433805209</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7">
+      <c r="B51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51">
+        <v>697</v>
+      </c>
+      <c r="E51">
+        <v>1366689148195.02</v>
+      </c>
+      <c r="F51">
+        <v>4381084.5789303798</v>
+      </c>
+      <c r="G51">
+        <v>12319.8361186564</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52">
+        <v>4418</v>
+      </c>
+      <c r="E52">
+        <v>108282.88</v>
+      </c>
+      <c r="F52">
+        <v>31050.973845322402</v>
+      </c>
+      <c r="G52">
+        <v>13.775443353742</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53">
+        <v>697</v>
+      </c>
+      <c r="E53">
+        <v>111883.3</v>
+      </c>
+      <c r="F53">
+        <v>23597.594605497299</v>
+      </c>
+      <c r="G53">
+        <v>66.357654844727094</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="B54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54">
+        <v>697</v>
+      </c>
+      <c r="E54">
+        <v>112113.54</v>
+      </c>
+      <c r="F54">
+        <v>23592.333451406401</v>
+      </c>
+      <c r="G54">
+        <v>66.342860207685206</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55">
+        <v>697</v>
+      </c>
+      <c r="E55">
+        <v>111836.95</v>
+      </c>
+      <c r="F55">
+        <v>23597.618816895101</v>
+      </c>
+      <c r="G55">
+        <v>66.357722928428203</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="B56" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56">
+        <v>697</v>
+      </c>
+      <c r="E56">
+        <v>112330.02</v>
+      </c>
+      <c r="F56">
+        <v>23602.4284708345</v>
+      </c>
+      <c r="G56">
+        <v>66.371247923724098</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7">
+      <c r="B57" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57">
+        <v>697</v>
+      </c>
+      <c r="E57">
+        <v>3268.56</v>
+      </c>
+      <c r="F57">
+        <v>878.84838921789606</v>
+      </c>
+      <c r="G57">
+        <v>2.4713670629369799</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58">
+        <v>4418</v>
+      </c>
+      <c r="E58">
+        <v>2711.53</v>
+      </c>
+      <c r="F58">
+        <v>977.72942189049604</v>
+      </c>
+      <c r="G58">
+        <v>0.43375954434254699</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7">
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59">
+        <v>697</v>
+      </c>
+      <c r="E59">
+        <v>2855.75</v>
+      </c>
+      <c r="F59">
+        <v>809.66877235262302</v>
+      </c>
+      <c r="G59">
+        <v>2.2768304071895802</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="B60" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60">
+        <v>697</v>
+      </c>
+      <c r="E60">
+        <v>7116.72</v>
+      </c>
+      <c r="F60">
+        <v>1563.6058591854301</v>
+      </c>
+      <c r="G60">
+        <v>4.3969404361598903</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61">
+        <v>697</v>
+      </c>
+      <c r="E61">
+        <v>2865.19</v>
+      </c>
+      <c r="F61">
+        <v>812.278312597786</v>
+      </c>
+      <c r="G61">
+        <v>2.2841685691415501</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7">
+      <c r="B62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" t="s">
+        <v>111</v>
+      </c>
+      <c r="D62">
+        <v>697</v>
+      </c>
+      <c r="E62">
+        <v>115382.1</v>
+      </c>
+      <c r="F62">
+        <v>24144.1509271096</v>
+      </c>
+      <c r="G62">
+        <v>67.894599450695495</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" t="s">
+        <v>111</v>
+      </c>
+      <c r="D63">
+        <v>697</v>
+      </c>
+      <c r="E63">
+        <v>114748.48</v>
+      </c>
+      <c r="F63">
+        <v>24085.468040141601</v>
+      </c>
+      <c r="G63">
+        <v>67.729580141574601</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7">
+      <c r="B64" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" t="s">
+        <v>111</v>
+      </c>
+      <c r="D64">
+        <v>697</v>
+      </c>
+      <c r="E64">
+        <v>119446.74</v>
+      </c>
+      <c r="F64">
+        <v>24284.8306194078</v>
+      </c>
+      <c r="G64">
+        <v>68.290198011534201</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="B65" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" t="s">
+        <v>111</v>
+      </c>
+      <c r="D65">
+        <v>697</v>
+      </c>
+      <c r="E65">
+        <v>114692.7</v>
+      </c>
+      <c r="F65">
+        <v>24084.661474798198</v>
+      </c>
+      <c r="G65">
+        <v>67.727312038169998</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7">
+      <c r="B66" t="s">
+        <v>113</v>
+      </c>
+      <c r="C66" t="s">
+        <v>111</v>
+      </c>
+      <c r="D66">
+        <v>4418</v>
+      </c>
+      <c r="E66">
+        <v>110994.41</v>
+      </c>
+      <c r="F66">
+        <v>31769.6453590848</v>
+      </c>
+      <c r="G66">
+        <v>14.094274536850699</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7">
+      <c r="B67" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67">
+        <v>697</v>
+      </c>
+      <c r="E67">
+        <v>577.15</v>
+      </c>
+      <c r="F67">
+        <v>1276.43662844707</v>
+      </c>
+      <c r="G67">
+        <v>3.5894057270534501</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7">
+      <c r="B68" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" t="s">
+        <v>112</v>
+      </c>
+      <c r="D68">
+        <v>4418</v>
+      </c>
+      <c r="E68">
+        <v>489.85</v>
+      </c>
+      <c r="F68">
+        <v>786.935533612276</v>
+      </c>
+      <c r="G68">
+        <v>0.34911580938887699</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7">
+      <c r="B69" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" t="s">
+        <v>112</v>
+      </c>
+      <c r="D69">
+        <v>697</v>
+      </c>
+      <c r="E69">
+        <v>445.51</v>
+      </c>
+      <c r="F69">
+        <v>404.09486588419003</v>
+      </c>
+      <c r="G69">
+        <v>1.13633563433718</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70" t="s">
+        <v>114</v>
+      </c>
+      <c r="C70" t="s">
+        <v>112</v>
+      </c>
+      <c r="D70">
+        <v>697</v>
+      </c>
+      <c r="E70">
+        <v>1302.0999999999999</v>
+      </c>
+      <c r="F70">
+        <v>1085.8462686391899</v>
+      </c>
+      <c r="G70">
+        <v>3.0534557912952698</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71">
+        <v>697</v>
+      </c>
+      <c r="E71">
+        <v>607.49</v>
+      </c>
+      <c r="F71">
+        <v>1363.9542754398201</v>
+      </c>
+      <c r="G71">
+        <v>3.8355098706772401</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
@@ -6776,7 +8180,7 @@
     <row r="2" spans="1:35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1">
         <v>3416</v>
@@ -6795,7 +8199,7 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1">
         <v>3636</v>
@@ -6814,7 +8218,7 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="1">
         <v>3719</v>
@@ -6833,7 +8237,7 @@
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X2" s="1">
         <v>3741</v>
@@ -6852,7 +8256,7 @@
       </c>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AE2" s="1">
         <v>3762</v>
@@ -6872,24 +8276,24 @@
     </row>
     <row r="3" spans="1:35">
       <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
+      <c r="Y3" t="s">
         <v>38</v>
       </c>
-      <c r="R3" t="s">
+      <c r="AF3" t="s">
         <v>39</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>1171</v>
@@ -6907,7 +8311,7 @@
         <v>11859.855330136401</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J4">
         <v>1225</v>
@@ -6925,7 +8329,7 @@
         <v>6201.9711732639398</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q4">
         <v>1252</v>
@@ -6943,7 +8347,7 @@
         <v>5289.6022753607704</v>
       </c>
       <c r="W4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="X4">
         <v>1260</v>
@@ -6961,7 +8365,7 @@
         <v>878.58458178384899</v>
       </c>
       <c r="AD4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AE4">
         <v>1268</v>
@@ -6981,7 +8385,7 @@
     </row>
     <row r="5" spans="1:35">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>4265</v>
@@ -6999,7 +8403,7 @@
         <v>6146.8739335056098</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J5">
         <v>4265</v>
@@ -7017,7 +8421,7 @@
         <v>2439.4270167761001</v>
       </c>
       <c r="P5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q5">
         <v>4265</v>
@@ -7035,7 +8439,7 @@
         <v>1638.6189707383401</v>
       </c>
       <c r="W5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X5">
         <v>4265</v>
@@ -7053,7 +8457,7 @@
         <v>291.52680657542197</v>
       </c>
       <c r="AD5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AE5">
         <v>4265</v>
@@ -7073,7 +8477,7 @@
     </row>
     <row r="6" spans="1:35">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6">
         <v>221</v>
@@ -7091,7 +8495,7 @@
         <v>5685.7883881938797</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J6">
         <v>287</v>
@@ -7109,7 +8513,7 @@
         <v>2140.0590929953801</v>
       </c>
       <c r="P6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q6">
         <v>328</v>
@@ -7127,7 +8531,7 @@
         <v>1345.79345830015</v>
       </c>
       <c r="W6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="X6">
         <v>337</v>
@@ -7145,7 +8549,7 @@
         <v>252.32218606597999</v>
       </c>
       <c r="AD6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AE6">
         <v>346</v>
@@ -7165,7 +8569,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>184</v>
@@ -7183,7 +8587,7 @@
         <v>5672.1373278576502</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J7">
         <v>184</v>
@@ -7201,7 +8605,7 @@
         <v>2120.6273310420502</v>
       </c>
       <c r="P7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q7">
         <v>184</v>
@@ -7219,7 +8623,7 @@
         <v>979.27852616543896</v>
       </c>
       <c r="W7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="X7">
         <v>184</v>
@@ -7237,7 +8641,7 @@
         <v>228.494655351375</v>
       </c>
       <c r="AD7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AE7">
         <v>184</v>
@@ -7257,7 +8661,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>18</v>
@@ -7275,7 +8679,7 @@
         <v>5552.3544902354397</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J8">
         <v>18</v>
@@ -7293,7 +8697,7 @@
         <v>2081.2161639765</v>
       </c>
       <c r="P8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q8">
         <v>18</v>
@@ -7311,7 +8715,7 @@
         <v>1056.5895793473901</v>
       </c>
       <c r="W8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="X8">
         <v>18</v>
@@ -7329,7 +8733,7 @@
         <v>260.33175331305699</v>
       </c>
       <c r="AD8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AE8">
         <v>18</v>
@@ -7349,12 +8753,12 @@
     </row>
     <row r="12" spans="1:35">
       <c r="D12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:35">
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13">
         <v>10193.3824</v>
@@ -7362,7 +8766,7 @@
     </row>
     <row r="14" spans="1:35">
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>5539.2927</v>
@@ -7370,7 +8774,7 @@
     </row>
     <row r="15" spans="1:35">
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15">
         <v>5303.5681999999997</v>
@@ -7378,7 +8782,7 @@
     </row>
     <row r="16" spans="1:35">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>5287.3666999999996</v>
@@ -7386,7 +8790,7 @@
     </row>
     <row r="17" spans="2:9">
       <c r="B17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D17">
         <v>5153.8462</v>
@@ -7394,15 +8798,15 @@
     </row>
     <row r="30" spans="2:9">
       <c r="D30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31">
         <v>3805</v>
@@ -7426,7 +8830,7 @@
     </row>
     <row r="32" spans="2:9">
       <c r="B32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32">
         <v>1282</v>
@@ -7450,7 +8854,7 @@
     </row>
     <row r="33" spans="2:9">
       <c r="B33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C33">
         <v>4265</v>
@@ -7474,7 +8878,7 @@
     </row>
     <row r="34" spans="2:9">
       <c r="B34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C34">
         <v>364</v>
@@ -7498,7 +8902,7 @@
     </row>
     <row r="35" spans="2:9">
       <c r="B35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C35">
         <v>184</v>
@@ -7522,7 +8926,7 @@
     </row>
     <row r="36" spans="2:9">
       <c r="B36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C36">
         <v>18</v>
@@ -7542,7 +8946,7 @@
     </row>
     <row r="47" spans="2:9">
       <c r="I47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="2:9">
@@ -7602,27 +9006,27 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" t="s">
-        <v>54</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" t="s">
         <v>53</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>3654</v>
@@ -7647,7 +9051,7 @@
         <v>164.97139999999999</v>
       </c>
       <c r="S2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T2">
         <v>3654</v>
@@ -7668,7 +9072,7 @@
         <v>291.47390000000001</v>
       </c>
       <c r="AA2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AB2">
         <v>3654</v>
@@ -7688,7 +9092,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>541</v>
@@ -7713,7 +9117,7 @@
         <v>120.2688</v>
       </c>
       <c r="S3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T3">
         <v>541</v>
@@ -7734,7 +9138,7 @@
         <v>251.53710000000001</v>
       </c>
       <c r="AA3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AB3">
         <v>541</v>
@@ -7763,7 +9167,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -7771,7 +9175,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -7790,18 +9194,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="2:16">
@@ -7809,7 +9213,7 @@
         <v>0.05</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>3994</v>
@@ -7827,7 +9231,7 @@
         <v>168.39603274311301</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L3">
         <v>13</v>
@@ -7850,7 +9254,7 @@
         <v>0.1</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <v>4355</v>
@@ -7868,7 +9272,7 @@
         <v>168.43765748429001</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L4">
         <v>4121</v>
@@ -7891,7 +9295,7 @@
         <v>0.25</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>4265</v>
@@ -7909,7 +9313,7 @@
         <v>164.99423393662599</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L5">
         <v>4355</v>
@@ -7932,7 +9336,7 @@
         <v>0.5</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>4368</v>
@@ -7950,7 +9354,7 @@
         <v>147.92409587328299</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L6">
         <v>4265</v>
@@ -7973,7 +9377,7 @@
         <v>0.75</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7">
         <v>4366</v>
@@ -7991,7 +9395,7 @@
         <v>111.48480722206899</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L7">
         <v>4368</v>
@@ -8014,7 +9418,7 @@
         <v>0.9</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8">
         <v>4340</v>
@@ -8032,7 +9436,7 @@
         <v>67.271245778883895</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L8">
         <v>4366</v>
@@ -8055,7 +9459,7 @@
         <v>0.95</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9">
         <v>3986</v>
@@ -8073,7 +9477,7 @@
         <v>41.595746391112598</v>
       </c>
       <c r="K9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L9">
         <v>4113</v>
@@ -8093,7 +9497,7 @@
     </row>
     <row r="10" spans="2:16">
       <c r="K10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L10">
         <v>20</v>
@@ -8113,7 +9517,7 @@
     </row>
     <row r="11" spans="2:16">
       <c r="K11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L11">
         <v>22</v>
@@ -8133,7 +9537,7 @@
     </row>
     <row r="12" spans="2:16">
       <c r="K12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L12">
         <v>4340</v>
@@ -8175,7 +9579,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -8235,7 +9639,7 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -9873,43 +11277,43 @@
   <sheetData>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" t="s">
+        <v>91</v>
+      </c>
+      <c r="O4" t="s">
         <v>92</v>
       </c>
-      <c r="K4" t="s">
+      <c r="Q4" t="s">
         <v>93</v>
       </c>
-      <c r="O4" t="s">
+      <c r="U4" t="s">
         <v>94</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>95</v>
-      </c>
-      <c r="U4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5">
         <v>2788</v>
@@ -9924,7 +11328,7 @@
         <v>0.87500761976709396</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J5">
         <v>2788</v>
@@ -9939,7 +11343,7 @@
         <v>4.4534870113327001</v>
       </c>
       <c r="O5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P5">
         <v>2788</v>
@@ -9960,10 +11364,10 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>697</v>
@@ -9978,7 +11382,7 @@
         <v>2.1774689791695301</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J6">
         <v>697</v>
@@ -9993,7 +11397,7 @@
         <v>0.70287368834331299</v>
       </c>
       <c r="O6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P6">
         <v>697</v>
@@ -10014,10 +11418,10 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>88</v>
@@ -10032,7 +11436,7 @@
         <v>91.185604585222904</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J7">
         <v>88</v>
@@ -10047,7 +11451,7 @@
         <v>3.8532873209707099</v>
       </c>
       <c r="O7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P7">
         <v>88</v>
@@ -10068,10 +11472,10 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -10086,7 +11490,7 @@
         <v>468.412819286949</v>
       </c>
       <c r="I8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J8">
         <v>30</v>
@@ -10101,7 +11505,7 @@
         <v>5.1971971990608496</v>
       </c>
       <c r="O8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P8">
         <v>30</v>
@@ -10122,10 +11526,10 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9">
         <v>26</v>
@@ -10140,7 +11544,7 @@
         <v>8729.2909631326202</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J9">
         <v>26</v>
@@ -10155,7 +11559,7 @@
         <v>2.9903048145519602</v>
       </c>
       <c r="O9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P9">
         <v>26</v>
@@ -10201,27 +11605,27 @@
   <sheetData>
     <row r="1" spans="2:31">
       <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" t="s">
         <v>102</v>
       </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>104</v>
       </c>
-      <c r="S1" t="s">
+      <c r="X1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC1" t="s">
         <v>106</v>
-      </c>
-      <c r="X1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="2:31">
       <c r="B2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>5493</v>
@@ -10236,7 +11640,7 @@
         <v>9.0660788072870493E-2</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H2">
         <v>5493</v>
@@ -10251,7 +11655,7 @@
         <v>8.6480739509190399E-2</v>
       </c>
       <c r="L2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M2">
         <v>5493</v>
@@ -10266,7 +11670,7 @@
         <v>5.37763105519561E-2</v>
       </c>
       <c r="Q2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R2">
         <v>5493</v>
@@ -10281,7 +11685,7 @@
         <v>6.0647182095143602E-2</v>
       </c>
       <c r="V2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="W2">
         <v>5493</v>
@@ -10296,7 +11700,7 @@
         <v>3.5276286917571E-5</v>
       </c>
       <c r="AA2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AB2">
         <v>5493</v>
@@ -10313,7 +11717,7 @@
     </row>
     <row r="3" spans="2:31">
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3">
         <v>5494</v>
@@ -10328,7 +11732,7 @@
         <v>9.0643281831517597E-2</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H3">
         <v>5494</v>
@@ -10343,7 +11747,7 @@
         <v>8.6463884836398094E-2</v>
       </c>
       <c r="L3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M3">
         <v>5494</v>
@@ -10358,7 +11762,7 @@
         <v>5.4936057568734903E-2</v>
       </c>
       <c r="Q3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R3">
         <v>5494</v>
@@ -10373,7 +11777,7 @@
         <v>6.1087659756118198E-2</v>
       </c>
       <c r="V3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="W3">
         <v>5494</v>
@@ -10388,7 +11792,7 @@
         <v>2.7060472417163398E-4</v>
       </c>
       <c r="AA3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AB3">
         <v>5494</v>
@@ -10405,7 +11809,7 @@
     </row>
     <row r="4" spans="2:31">
       <c r="B4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>5497</v>
@@ -10420,7 +11824,7 @@
         <v>9.0590238488394106E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H4">
         <v>5497</v>
@@ -10435,7 +11839,7 @@
         <v>8.6412863831662801E-2</v>
       </c>
       <c r="L4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M4">
         <v>5497</v>
@@ -10450,7 +11854,7 @@
         <v>5.9015454219437102E-2</v>
       </c>
       <c r="Q4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R4">
         <v>5497</v>
@@ -10465,7 +11869,7 @@
         <v>6.40072217753508E-2</v>
       </c>
       <c r="V4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W4">
         <v>5497</v>
@@ -10480,7 +11884,7 @@
         <v>1.2530401635196899E-3</v>
       </c>
       <c r="AA4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AB4">
         <v>5497</v>
@@ -10497,7 +11901,7 @@
     </row>
     <row r="5" spans="2:31">
       <c r="B5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5">
         <v>5499</v>
@@ -10512,7 +11916,7 @@
         <v>9.0550721174100998E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H5">
         <v>5499</v>
@@ -10527,7 +11931,7 @@
         <v>8.6375988665648704E-2</v>
       </c>
       <c r="L5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M5">
         <v>5499</v>
@@ -10542,7 +11946,7 @@
         <v>6.4162376924033704E-2</v>
       </c>
       <c r="Q5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R5">
         <v>5499</v>
@@ -10557,7 +11961,7 @@
         <v>7.3094059343264101E-2</v>
       </c>
       <c r="V5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="W5">
         <v>5499</v>
@@ -10572,7 +11976,7 @@
         <v>2.17302766911914E-3</v>
       </c>
       <c r="AA5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AB5">
         <v>5499</v>
@@ -10589,7 +11993,7 @@
     </row>
     <row r="6" spans="2:31">
       <c r="B6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>5501</v>
@@ -10604,7 +12008,7 @@
         <v>9.0507465978203194E-2</v>
       </c>
       <c r="G6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H6">
         <v>5501</v>
@@ -10619,7 +12023,7 @@
         <v>8.6335322657928495E-2</v>
       </c>
       <c r="L6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M6">
         <v>5501</v>
@@ -10634,7 +12038,7 @@
         <v>7.1296533036076207E-2</v>
       </c>
       <c r="Q6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R6">
         <v>5501</v>
@@ -10649,7 +12053,7 @@
         <v>9.1585406147622797E-2</v>
       </c>
       <c r="V6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="W6">
         <v>5501</v>
@@ -10664,7 +12068,7 @@
         <v>2.9684809627319102E-3</v>
       </c>
       <c r="AA6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AB6">
         <v>5501</v>

</xml_diff>

<commit_message>
Reverting reciprocal confidence stuff.. it didn't make a difference and can't be explained
</commit_message>
<xml_diff>
--- a/write-ups/cikm/performance.xlsx
+++ b/write-ups/cikm/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Change with Epochlength" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="126">
   <si>
     <t>MinSupp</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Epoch in Hrs</t>
   </si>
   <si>
-    <t>Avg Millis Mining</t>
-  </si>
-  <si>
     <t>Avg Support</t>
   </si>
   <si>
@@ -389,6 +386,24 @@
   </si>
   <si>
     <t>Mean number of distinct terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1351504800, 1354359600, file:///home/yaboulna/fim_out/lcm_closed_cikm/bg_1hr+1hr_ngram5-relsupp10_oct29-nov, 3600/3600, /home/yaboulna/fimi/lcm53/lcm Cf, &gt;10, 5] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select args, count(*), round(cast(avg(value) as numeric), 2), stddev(value),  (1.96 * stddev(value) / count(*)) as err from perf_mon where args like '%bg_1hr%&gt;10, 5]' and key='WallMillisMining' group by args;</t>
+  </si>
+  <si>
+    <t>Wall clock runtime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1351504800, 1357038000, file:///home/yaboulna/fim_out/lcm_closed_cikm_len2+/16hr+8hr_ngram5-relsupp10_oct29-nov-dec, 57600/28800, /home/yaboulna/fimi/lcm53/lcm CfI, &gt;10, 5]          </t>
+  </si>
+  <si>
+    <t>16 hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1351504800, 1357038000, file:///home/yaboulna/fim_out/lcm_closed_cikm_len2+/max_16hr+8hr_ngram5-relsupp10_oct29-nov-dec, 57600/28800, /home/yaboulna/fimi/fp-zhu/fim_maximal, &gt;10, 5] </t>
   </si>
 </sst>
 </file>
@@ -450,8 +465,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="221">
+  <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -679,7 +712,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="221">
+  <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -790,6 +823,15 @@
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -900,6 +942,15 @@
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -921,31 +972,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Avg Wall Clock Run Time</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -961,7 +988,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg Millis Mining</c:v>
+                  <c:v>Wall clock runtime</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -969,9 +996,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$B$2:$B$8</c:f>
+              <c:f>'Change with Epochlength'!$B$2:$B$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5 min</c:v>
                 </c:pt>
@@ -985,12 +1012,15 @@
                   <c:v>8 hr</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>16 hr</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1 day</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1 week</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>4 weeks</c:v>
                 </c:pt>
               </c:strCache>
@@ -998,30 +1028,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$D$2:$D$8</c:f>
+              <c:f>'Change with Epochlength'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>72.9230759806233</c:v>
+                  <c:v>72.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>165.23778944777</c:v>
+                  <c:v>165.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>489.851223918062</c:v>
+                  <c:v>489.85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3924.68213097107</c:v>
+                  <c:v>3924.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12693.2167072295</c:v>
+                  <c:v>8606.360000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>166043.038536024</c:v>
+                  <c:v>12693.22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>635074.7902145</c:v>
+                  <c:v>166043.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>635074.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1425,10 +1458,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with ngram len'!$R$2:$R$6</c:f>
+              <c:f>'Change with ngram len'!$R$2:$R$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1302.1</c:v>
                 </c:pt>
@@ -1442,6 +1475,9 @@
                   <c:v>445.51</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>369.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>489.85</c:v>
                 </c:pt>
               </c:numCache>
@@ -1591,7 +1627,7 @@
                   <c:v>445.51</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>489.85</c:v>
+                  <c:v>369.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2977,10 +3013,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$P$2:$P$8</c:f>
+              <c:f>'Change with Epochlength'!$P$2:$P$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>71970.5784444999</c:v>
                 </c:pt>
@@ -2993,13 +3029,13 @@
                 <c:pt idx="3">
                   <c:v>3.08354324231465E6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>7.49974681081081E6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3.36463622666667E7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>9.49602949E7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3573,7 +3609,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$C$35:$C$56</c:f>
+              <c:f>'Change with Epochlength'!$C$36:$C$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -3648,7 +3684,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$D$35:$D$56</c:f>
+              <c:f>'Change with Epochlength'!$D$36:$D$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -3657,6 +3693,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3924.682131</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8606.360000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12693.21671</c:v>
@@ -3790,10 +3829,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$I$2:$I$8</c:f>
+              <c:f>'Change with Epochlength'!$I$2:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>4.3858</c:v>
                 </c:pt>
@@ -3806,13 +3845,13 @@
                 <c:pt idx="3">
                   <c:v>158.8553</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>476.954</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3336.4634</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>13410.1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3949,10 +3988,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$H$2:$H$8</c:f>
+              <c:f>'Change with Epochlength'!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>9311.3487</c:v>
                 </c:pt>
@@ -3965,13 +4004,13 @@
                 <c:pt idx="3">
                   <c:v>887997.1609</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2.6646958E6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.84375102E7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7.46542102E7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3995,10 +4034,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$I$2:$I$8</c:f>
+              <c:f>'Change with Epochlength'!$I$2:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>4.3858</c:v>
                 </c:pt>
@@ -4011,13 +4050,13 @@
                 <c:pt idx="3">
                   <c:v>158.8553</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>476.954</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3336.4634</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>13410.1</c:v>
                 </c:pt>
               </c:numCache>
@@ -4146,10 +4185,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$C$2:$C$6</c:f>
+              <c:f>'Change with Epochlength'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1512.0237</c:v>
                 </c:pt>
@@ -4162,7 +4201,7 @@
                 <c:pt idx="3">
                   <c:v>1552.1978</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1426.5217</c:v>
                 </c:pt>
               </c:numCache>
@@ -4178,7 +4217,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg Millis Mining</c:v>
+                  <c:v>Wall clock runtime</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4186,24 +4225,27 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$D$2:$D$6</c:f>
+              <c:f>'Change with Epochlength'!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>72.9230759806233</c:v>
+                  <c:v>72.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>165.23778944777</c:v>
+                  <c:v>165.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>489.851223918062</c:v>
+                  <c:v>489.85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3924.68213097107</c:v>
+                  <c:v>3924.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12693.2167072295</c:v>
+                  <c:v>8606.360000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12693.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4298,7 +4340,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$F$89</c:f>
+              <c:f>'Change with Epochlength'!$F$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4312,7 +4354,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$E$90:$E$95</c:f>
+              <c:f>'Change with Epochlength'!$E$91:$E$96</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4338,7 +4380,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$F$90:$F$95</c:f>
+              <c:f>'Change with Epochlength'!$F$91:$F$96</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4367,7 +4409,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$G$89</c:f>
+              <c:f>'Change with Epochlength'!$G$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4381,7 +4423,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$E$90:$E$95</c:f>
+              <c:f>'Change with Epochlength'!$E$91:$E$96</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4407,7 +4449,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$G$90:$G$95</c:f>
+              <c:f>'Change with Epochlength'!$G$91:$G$96</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4436,7 +4478,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$I$89</c:f>
+              <c:f>'Change with Epochlength'!$I$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4450,7 +4492,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$E$90:$E$95</c:f>
+              <c:f>'Change with Epochlength'!$E$91:$E$96</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4476,7 +4518,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$I$90:$I$95</c:f>
+              <c:f>'Change with Epochlength'!$I$91:$I$96</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4488,6 +4530,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22162.1795</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50074.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>86286.6761</c:v>
@@ -4549,6 +4594,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4608,6 +4654,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4621,7 +4668,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$G$89</c:f>
+              <c:f>'Change with Epochlength'!$G$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4638,7 +4685,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$E$90:$E$95</c:f>
+              <c:f>'Change with Epochlength'!$E$91:$E$96</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4664,7 +4711,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$G$90:$G$94</c:f>
+              <c:f>'Change with Epochlength'!$G$91:$G$95</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4690,7 +4737,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$H$89</c:f>
+              <c:f>'Change with Epochlength'!$H$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4707,7 +4754,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$E$90:$E$95</c:f>
+              <c:f>'Change with Epochlength'!$E$91:$E$96</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4733,7 +4780,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$H$90:$H$94</c:f>
+              <c:f>'Change with Epochlength'!$H$91:$H$95</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4759,7 +4806,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$I$89</c:f>
+              <c:f>'Change with Epochlength'!$I$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4776,7 +4823,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Change with Epochlength'!$E$90:$E$95</c:f>
+              <c:f>'Change with Epochlength'!$E$91:$E$96</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4802,7 +4849,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Change with Epochlength'!$I$90:$I$94</c:f>
+              <c:f>'Change with Epochlength'!$I$91:$I$95</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4814,6 +4861,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22162.1795</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50074.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>86286.6761</c:v>
@@ -4877,6 +4927,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4890,6 +4941,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5029,13 +5081,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5059,13 +5111,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5089,13 +5141,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5119,13 +5171,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5149,13 +5201,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5179,13 +5231,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5209,13 +5261,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5239,13 +5291,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>117</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6035,10 +6087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S95"/>
+  <dimension ref="A1:S96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6057,25 +6109,25 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -6093,7 +6145,7 @@
         <v>5</v>
       </c>
       <c r="P1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -6101,19 +6153,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1512.0237</v>
       </c>
       <c r="D2">
-        <v>72.923075980623295</v>
+        <v>72.92</v>
       </c>
       <c r="E2">
         <v>359.26363005089399</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F8" si="0">1.96*E2/G2</f>
+        <f t="shared" ref="F2:F9" si="0">1.96*E2/G2</f>
         <v>1.6379546752727427E-2</v>
       </c>
       <c r="G2">
@@ -6155,13 +6207,13 @@
     </row>
     <row r="3" spans="1:19">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>6409.9687999999996</v>
       </c>
       <c r="D3">
-        <v>165.23778944777001</v>
+        <v>165.24</v>
       </c>
       <c r="E3">
         <v>492.91101657370399</v>
@@ -6209,13 +6261,13 @@
     </row>
     <row r="4" spans="1:19">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>1762.973</v>
       </c>
       <c r="D4">
-        <v>489.85122391806198</v>
+        <v>489.85</v>
       </c>
       <c r="E4">
         <v>786.935533612276</v>
@@ -6263,13 +6315,13 @@
     </row>
     <row r="5" spans="1:19">
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1552.1977999999999</v>
       </c>
       <c r="D5">
-        <v>3924.6821309710699</v>
+        <v>3924.68</v>
       </c>
       <c r="E5">
         <v>1521.31462762654</v>
@@ -6316,703 +6368,740 @@
       </c>
     </row>
     <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>1426.5217</v>
+        <v>124</v>
       </c>
       <c r="D6">
-        <v>12693.2167072295</v>
+        <v>8606.36</v>
       </c>
       <c r="E6">
-        <v>4250.6487382266796</v>
+        <v>2582.8536187414002</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>27.31564435057145</v>
-      </c>
-      <c r="G6">
-        <v>305</v>
-      </c>
-      <c r="H6">
-        <v>2664695.7999999998</v>
-      </c>
-      <c r="I6" s="1">
-        <v>476.95400000000001</v>
-      </c>
-      <c r="J6">
-        <v>68.864076585716703</v>
-      </c>
-      <c r="K6">
-        <v>305</v>
-      </c>
-      <c r="L6">
-        <v>477.39663472166598</v>
-      </c>
-      <c r="M6">
-        <v>476.51156199964601</v>
-      </c>
-      <c r="O6">
-        <v>185</v>
-      </c>
-      <c r="P6">
-        <v>7499746.81081081</v>
-      </c>
-      <c r="Q6">
-        <v>1171877.30432764</v>
-      </c>
-      <c r="R6">
-        <v>7487331.2458568504</v>
-      </c>
-      <c r="S6">
-        <v>7512162.3757647704</v>
+        <v>26.230016024520001</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>3242.7777999999998</v>
+        <v>1426.5217</v>
       </c>
       <c r="D7">
-        <v>166043.03853602399</v>
+        <v>12693.22</v>
       </c>
       <c r="E7">
-        <v>61021.062936321301</v>
+        <v>4250.6487382266796</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>2917.1044720777986</v>
+        <v>27.31564435057145</v>
       </c>
       <c r="G7">
-        <v>41</v>
+        <v>305</v>
       </c>
       <c r="H7">
-        <v>18437510.199999999</v>
-      </c>
-      <c r="I7">
-        <v>3336.4634000000001</v>
+        <v>2664695.7999999998</v>
+      </c>
+      <c r="I7" s="1">
+        <v>476.95400000000001</v>
       </c>
       <c r="J7">
-        <v>251.03606290341801</v>
+        <v>68.864076585716703</v>
       </c>
       <c r="K7">
-        <v>41</v>
+        <v>305</v>
       </c>
       <c r="L7">
-        <v>3348.4641630070901</v>
+        <v>477.39663472166598</v>
       </c>
       <c r="M7">
-        <v>3324.4626662612</v>
+        <v>476.51156199964601</v>
       </c>
       <c r="O7">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="P7">
-        <v>33646362.266666703</v>
+        <v>7499746.81081081</v>
       </c>
       <c r="Q7">
-        <v>1171786.97335306</v>
+        <v>1171877.30432764</v>
       </c>
       <c r="R7">
-        <v>33493248.768815201</v>
+        <v>7487331.2458568504</v>
       </c>
       <c r="S7">
-        <v>33799475.764518097</v>
+        <v>7512162.3757647704</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>3242.7777999999998</v>
       </c>
       <c r="D8">
-        <v>635074.79021450004</v>
+        <v>166043.04</v>
       </c>
       <c r="E8">
+        <v>61021.062936321301</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2917.1044720777986</v>
+      </c>
+      <c r="G8">
+        <v>41</v>
+      </c>
+      <c r="H8">
+        <v>18437510.199999999</v>
+      </c>
+      <c r="I8">
+        <v>3336.4634000000001</v>
+      </c>
+      <c r="J8">
+        <v>251.03606290341801</v>
+      </c>
+      <c r="K8">
+        <v>41</v>
+      </c>
+      <c r="L8">
+        <v>3348.4641630070901</v>
+      </c>
+      <c r="M8">
+        <v>3324.4626662612</v>
+      </c>
+      <c r="O8">
+        <v>15</v>
+      </c>
+      <c r="P8">
+        <v>33646362.266666703</v>
+      </c>
+      <c r="Q8">
+        <v>1171786.97335306</v>
+      </c>
+      <c r="R8">
+        <v>33493248.768815201</v>
+      </c>
+      <c r="S8">
+        <v>33799475.764518097</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>635074.79</v>
+      </c>
+      <c r="E9">
         <v>171717.60344923401</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>33656.65027604987</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>10</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>74654210.200000003</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>13410.1</v>
       </c>
-      <c r="J8">
+      <c r="J9">
         <v>376.52606520369602</v>
       </c>
-      <c r="K8">
+      <c r="K9">
         <v>10</v>
       </c>
-      <c r="L8">
+      <c r="L9">
         <v>13483.8991087799</v>
       </c>
-      <c r="M8">
+      <c r="M9">
         <v>13336.3008912201</v>
       </c>
-      <c r="O8">
+      <c r="O9">
         <v>10</v>
       </c>
-      <c r="P8">
+      <c r="P9">
         <v>94960294.900000006</v>
       </c>
-      <c r="Q8">
+      <c r="Q9">
         <v>1854540.6462349601</v>
       </c>
-      <c r="R8">
+      <c r="R9">
         <v>94596804.933338001</v>
       </c>
-      <c r="S8">
+      <c r="S9">
         <v>95323784.8666621</v>
       </c>
     </row>
-    <row r="32" spans="5:5">
-      <c r="E32" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="33" spans="2:12">
-      <c r="B33">
-        <v>300</v>
-      </c>
-      <c r="C33">
-        <f>B33/3600</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D33" s="1">
-        <v>72.923075979999993</v>
-      </c>
-      <c r="E33">
-        <v>1662.2942</v>
-      </c>
-      <c r="I33" t="s">
-        <v>25</v>
+      <c r="E33" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="2:12">
       <c r="B34">
-        <v>900</v>
+        <v>300</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C38" si="1">B34/3600</f>
-        <v>0.25</v>
+        <f>B34/3600</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D34" s="1">
-        <v>165.2377894</v>
+        <v>72.923075979999993</v>
       </c>
       <c r="E34">
-        <v>7019.4350000000004</v>
-      </c>
-      <c r="H34">
-        <v>44063</v>
-      </c>
-      <c r="I34">
-        <v>9311.3487506524707</v>
-      </c>
-      <c r="J34">
-        <v>2336.7182062635202</v>
-      </c>
-      <c r="K34">
-        <v>9311.2448093029507</v>
-      </c>
-      <c r="L34">
-        <v>9311.4526920019998</v>
+        <v>1662.2942</v>
+      </c>
+      <c r="I34" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="2:12">
       <c r="B35">
+        <v>900</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C39" si="1">B35/3600</f>
+        <v>0.25</v>
+      </c>
+      <c r="D35" s="1">
+        <v>165.2377894</v>
+      </c>
+      <c r="E35">
+        <v>7019.4350000000004</v>
+      </c>
+      <c r="H35">
+        <v>44063</v>
+      </c>
+      <c r="I35">
+        <v>9311.3487506524707</v>
+      </c>
+      <c r="J35">
+        <v>2336.7182062635202</v>
+      </c>
+      <c r="K35">
+        <v>9311.2448093029507</v>
+      </c>
+      <c r="L35">
+        <v>9311.4526920019998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36">
         <v>3600</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D36" s="1">
         <v>489.85122389999998</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <v>1762.973</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>17672</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <v>27748.328315980099</v>
       </c>
-      <c r="J35">
+      <c r="J36">
         <v>8021.8856394166396</v>
       </c>
-      <c r="K35">
+      <c r="K36">
         <v>27747.4386093338</v>
       </c>
-      <c r="L35">
+      <c r="L36">
         <v>27749.218022626399</v>
       </c>
     </row>
-    <row r="36" spans="2:12">
-      <c r="B36">
+    <row r="37" spans="2:12">
+      <c r="B37">
         <v>28800</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D37" s="1">
         <v>3924.682131</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <v>6062.125</v>
       </c>
-      <c r="H36">
+      <c r="H37">
         <v>4418</v>
       </c>
-      <c r="I36">
+      <c r="I37">
         <v>110994.410366682</v>
       </c>
-      <c r="J36">
+      <c r="J37">
         <v>31769.6453590848</v>
       </c>
-      <c r="K36">
+      <c r="K37">
         <v>110980.316092145</v>
       </c>
-      <c r="L36">
+      <c r="L37">
         <v>111008.504641219</v>
       </c>
     </row>
-    <row r="37" spans="2:12">
-      <c r="C37">
+    <row r="38" spans="2:12">
+      <c r="C38">
         <v>16</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="H37">
+      <c r="D38">
+        <v>8606.36</v>
+      </c>
+      <c r="H38">
         <v>553</v>
       </c>
-      <c r="I37">
+      <c r="I38">
         <v>887997.160940325</v>
       </c>
-      <c r="J37">
+      <c r="J38">
         <v>205533.12966613501</v>
       </c>
-      <c r="K37">
+      <c r="K38">
         <v>887268.68908834399</v>
       </c>
-      <c r="L37">
+      <c r="L38">
         <v>888725.63279230695</v>
       </c>
     </row>
-    <row r="38" spans="2:12">
-      <c r="B38">
+    <row r="39" spans="2:12">
+      <c r="B39">
         <v>86400</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D39" s="1">
         <v>12693.216710000001</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>1426.5217</v>
       </c>
-      <c r="H38">
+      <c r="H39">
         <v>185</v>
       </c>
-      <c r="I38">
+      <c r="I39">
         <v>2664695.7999999998</v>
       </c>
-      <c r="J38">
+      <c r="J39">
         <v>450348.83846423402</v>
       </c>
-      <c r="K38">
+      <c r="K39">
         <v>2659924.5366303199</v>
       </c>
-      <c r="L38">
+      <c r="L39">
         <v>2669467.0633696802</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12">
-      <c r="C39">
-        <f>C38+8</f>
-        <v>32</v>
-      </c>
-      <c r="H39">
-        <v>15</v>
-      </c>
-      <c r="I39">
-        <v>18437510.199999999</v>
-      </c>
-      <c r="J39">
-        <v>874753.14862742799</v>
-      </c>
-      <c r="K39">
-        <v>18323209.121912699</v>
-      </c>
-      <c r="L39">
-        <v>18551811.278087299</v>
       </c>
     </row>
     <row r="40" spans="2:12">
       <c r="C40">
-        <f t="shared" ref="C40:C56" si="2">C39+8</f>
-        <v>40</v>
+        <f>C39+8</f>
+        <v>32</v>
       </c>
       <c r="H40">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I40">
-        <v>74654210.200000003</v>
+        <v>18437510.199999999</v>
       </c>
       <c r="J40">
-        <v>2231284.86810969</v>
+        <v>874753.14862742799</v>
       </c>
       <c r="K40">
-        <v>74216878.365850493</v>
+        <v>18323209.121912699</v>
       </c>
       <c r="L40">
-        <v>75091542.034149498</v>
+        <v>18551811.278087299</v>
       </c>
     </row>
     <row r="41" spans="2:12">
       <c r="C41">
-        <f t="shared" si="2"/>
-        <v>48</v>
+        <f t="shared" ref="C41:C57" si="2">C40+8</f>
+        <v>40</v>
+      </c>
+      <c r="H41">
+        <v>10</v>
+      </c>
+      <c r="I41">
+        <v>74654210.200000003</v>
+      </c>
+      <c r="J41">
+        <v>2231284.86810969</v>
+      </c>
+      <c r="K41">
+        <v>74216878.365850493</v>
+      </c>
+      <c r="L41">
+        <v>75091542.034149498</v>
       </c>
     </row>
     <row r="42" spans="2:12">
       <c r="C42">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="2:12">
       <c r="C43">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:12">
       <c r="C44">
         <f t="shared" si="2"/>
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="2:12">
       <c r="C45">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="2:12">
       <c r="C46">
         <f t="shared" si="2"/>
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="2:12">
       <c r="C47">
         <f t="shared" si="2"/>
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="2:12">
       <c r="C48">
         <f t="shared" si="2"/>
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="3:5">
       <c r="C49">
         <f t="shared" si="2"/>
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="3:5">
       <c r="C50">
         <f t="shared" si="2"/>
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="3:5">
       <c r="C51">
         <f t="shared" si="2"/>
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="3:5">
       <c r="C52">
         <f t="shared" si="2"/>
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="3:5">
       <c r="C53">
         <f t="shared" si="2"/>
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="3:5">
       <c r="C54">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="3:5">
       <c r="C55">
         <f t="shared" si="2"/>
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="3:5">
       <c r="C56">
         <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5">
+      <c r="C57">
+        <f t="shared" si="2"/>
         <v>168</v>
       </c>
-      <c r="D56">
+      <c r="D57">
         <v>166043.03853602399</v>
       </c>
-      <c r="E56">
+      <c r="E57">
         <v>3242.7777999999998</v>
       </c>
     </row>
-    <row r="65" spans="2:7">
-      <c r="D65" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="66" spans="2:7">
-      <c r="B66" t="s">
-        <v>28</v>
-      </c>
-      <c r="C66">
-        <v>3805</v>
-      </c>
-      <c r="D66">
-        <v>1512.0237</v>
-      </c>
-      <c r="E66">
-        <v>971.68682911074995</v>
-      </c>
-      <c r="F66">
-        <v>1511.5231258383601</v>
-      </c>
-      <c r="G66">
-        <v>1512.5241803377301</v>
+      <c r="D66" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="2:7">
       <c r="B67" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C67">
-        <v>1282</v>
+        <v>3805</v>
       </c>
       <c r="D67">
-        <v>6409.9687999999996</v>
+        <v>1512.0237</v>
       </c>
       <c r="E67">
-        <v>5123.8223679853099</v>
+        <v>971.68682911074995</v>
       </c>
       <c r="F67">
-        <v>6402.1351857712598</v>
+        <v>1511.5231258383601</v>
       </c>
       <c r="G67">
-        <v>6417.8024117326404</v>
+        <v>1512.5241803377301</v>
       </c>
     </row>
     <row r="68" spans="2:7">
       <c r="B68" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C68">
-        <v>4265</v>
+        <v>1282</v>
       </c>
       <c r="D68">
-        <v>1762.973</v>
+        <v>6409.9687999999996</v>
       </c>
       <c r="E68">
-        <v>803.388243193123</v>
+        <v>5123.8223679853099</v>
       </c>
       <c r="F68">
-        <v>1762.6038356490801</v>
+        <v>6402.1351857712598</v>
       </c>
       <c r="G68">
-        <v>1763.3422370355599</v>
+        <v>6417.8024117326404</v>
       </c>
     </row>
     <row r="69" spans="2:7">
       <c r="B69" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C69">
-        <v>364</v>
+        <v>4265</v>
       </c>
       <c r="D69">
-        <v>1552.1977999999999</v>
+        <v>1762.973</v>
       </c>
       <c r="E69">
-        <v>997.73274901270895</v>
+        <v>803.388243193123</v>
       </c>
       <c r="F69">
-        <v>1546.8253950877299</v>
+        <v>1762.6038356490801</v>
       </c>
       <c r="G69">
-        <v>1557.5702093078701</v>
+        <v>1763.3422370355599</v>
       </c>
     </row>
     <row r="70" spans="2:7">
       <c r="B70" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C70">
-        <v>184</v>
+        <v>364</v>
       </c>
       <c r="D70">
-        <v>1426.5217</v>
+        <v>1552.1977999999999</v>
       </c>
       <c r="E70">
-        <v>1963.46851276452</v>
+        <v>997.73274901270895</v>
       </c>
       <c r="F70">
-        <v>1405.60653105968</v>
+        <v>1546.8253950877299</v>
       </c>
       <c r="G70">
-        <v>1447.4369472011899</v>
+        <v>1557.5702093078701</v>
       </c>
     </row>
     <row r="71" spans="2:7">
       <c r="B71" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C71">
+        <v>184</v>
+      </c>
+      <c r="D71">
+        <v>1426.5217</v>
+      </c>
+      <c r="E71">
+        <v>1963.46851276452</v>
+      </c>
+      <c r="F71">
+        <v>1405.60653105968</v>
+      </c>
+      <c r="G71">
+        <v>1447.4369472011899</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72">
         <v>18</v>
       </c>
-      <c r="D71">
+      <c r="D72">
         <v>3242.7777999999998</v>
       </c>
-      <c r="E71">
+      <c r="E72">
         <v>3902.5931131154298</v>
       </c>
-      <c r="F71">
+      <c r="F72">
         <v>2817.8287499052099</v>
       </c>
-      <c r="G71">
+      <c r="G72">
         <v>3667.7268056503499</v>
       </c>
     </row>
-    <row r="89" spans="5:9">
-      <c r="F89" t="s">
+    <row r="90" spans="5:14">
+      <c r="F90" t="s">
+        <v>85</v>
+      </c>
+      <c r="G90" t="s">
+        <v>84</v>
+      </c>
+      <c r="H90" t="s">
         <v>86</v>
       </c>
-      <c r="G89" t="s">
-        <v>85</v>
-      </c>
-      <c r="H89" t="s">
+      <c r="I90" t="s">
         <v>87</v>
       </c>
-      <c r="I89" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="5:9">
-      <c r="E90" t="s">
+    </row>
+    <row r="91" spans="5:14">
+      <c r="E91" t="s">
+        <v>18</v>
+      </c>
+      <c r="F91">
+        <v>6409.9687999999996</v>
+      </c>
+      <c r="G91">
+        <v>165.23778944777001</v>
+      </c>
+      <c r="H91">
+        <f>F91+G91</f>
+        <v>6575.2065894477701</v>
+      </c>
+      <c r="I91">
+        <v>1583.4784999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="5:14">
+      <c r="E92" t="s">
         <v>19</v>
       </c>
-      <c r="F90">
-        <v>6409.9687999999996</v>
-      </c>
-      <c r="G90">
-        <v>165.23778944777001</v>
-      </c>
-      <c r="H90">
-        <f>F90+G90</f>
-        <v>6575.2065894477701</v>
-      </c>
-      <c r="I90">
-        <v>1583.4784999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="5:9">
-      <c r="E91" t="s">
+      <c r="F92">
+        <v>1762.973</v>
+      </c>
+      <c r="G92">
+        <v>489.85122391806198</v>
+      </c>
+      <c r="H92">
+        <f t="shared" ref="H92:H96" si="3">F92+G92</f>
+        <v>2252.8242239180618</v>
+      </c>
+      <c r="I92">
+        <v>2390.0704999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="5:14">
+      <c r="E93" t="s">
         <v>20</v>
       </c>
-      <c r="F91">
-        <v>1762.973</v>
-      </c>
-      <c r="G91">
-        <v>489.85122391806198</v>
-      </c>
-      <c r="H91">
-        <f t="shared" ref="H91:H95" si="3">F91+G91</f>
-        <v>2252.8242239180618</v>
-      </c>
-      <c r="I91">
-        <v>2390.0704999999998</v>
-      </c>
-    </row>
-    <row r="92" spans="5:9">
-      <c r="E92" t="s">
-        <v>21</v>
-      </c>
-      <c r="F92">
+      <c r="F93">
         <v>1552.1977999999999</v>
       </c>
-      <c r="G92">
+      <c r="G93">
         <v>3924.6821309710699</v>
       </c>
-      <c r="H92">
+      <c r="H93">
         <f t="shared" si="3"/>
         <v>5476.8799309710703</v>
       </c>
-      <c r="I92">
+      <c r="I93">
         <v>22162.179499999998</v>
       </c>
     </row>
-    <row r="93" spans="5:9">
-      <c r="E93" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="94" spans="5:9">
+    <row r="94" spans="5:14">
       <c r="E94" t="s">
-        <v>22</v>
-      </c>
-      <c r="F94">
+        <v>88</v>
+      </c>
+      <c r="I94">
+        <v>50074.05</v>
+      </c>
+      <c r="J94" t="s">
+        <v>125</v>
+      </c>
+      <c r="K94">
+        <v>191</v>
+      </c>
+      <c r="L94">
+        <v>50074.05</v>
+      </c>
+      <c r="M94">
+        <v>10067.9771846607</v>
+      </c>
+      <c r="N94">
+        <v>103.31536796824599</v>
+      </c>
+    </row>
+    <row r="95" spans="5:14">
+      <c r="E95" t="s">
+        <v>21</v>
+      </c>
+      <c r="F95">
         <v>1426.5217</v>
       </c>
-      <c r="G94">
+      <c r="G95">
         <v>12693.2167072295</v>
       </c>
-      <c r="H94">
+      <c r="H95">
         <f t="shared" si="3"/>
         <v>14119.738407229499</v>
       </c>
-      <c r="I94">
+      <c r="I95">
         <v>86286.676099999997</v>
       </c>
     </row>
-    <row r="95" spans="5:9">
-      <c r="E95" t="s">
-        <v>23</v>
-      </c>
-      <c r="F95">
+    <row r="96" spans="5:14">
+      <c r="E96" t="s">
+        <v>22</v>
+      </c>
+      <c r="F96">
         <v>3242.7777999999998</v>
       </c>
-      <c r="G95">
+      <c r="G96">
         <v>166043.03853602399</v>
       </c>
-      <c r="H95">
+      <c r="H96">
         <f t="shared" si="3"/>
         <v>169285.816336024</v>
       </c>
-      <c r="I95">
+      <c r="I96">
         <v>868539.87250000006</v>
       </c>
     </row>
@@ -7032,8 +7121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7046,49 +7135,49 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
       <c r="J1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
         <v>119</v>
       </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" t="s">
-        <v>120</v>
-      </c>
       <c r="R1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -7135,10 +7224,10 @@
         <v>185.90600000000001</v>
       </c>
       <c r="O2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q2">
         <v>697</v>
@@ -7155,7 +7244,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7197,10 +7286,10 @@
         <v>557.68700000000001</v>
       </c>
       <c r="O3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q3">
         <v>697</v>
@@ -7217,7 +7306,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7259,10 +7348,10 @@
         <v>589.02</v>
       </c>
       <c r="O4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q4">
         <v>697</v>
@@ -7313,10 +7402,10 @@
         <v>589.12900000000002</v>
       </c>
       <c r="O5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q5">
         <v>697</v>
@@ -7373,30 +7462,52 @@
         <v>569.84799999999996</v>
       </c>
       <c r="O6" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="P6" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q6">
+        <v>793</v>
+      </c>
+      <c r="R6">
+        <v>369.48</v>
+      </c>
+      <c r="S6">
+        <v>112.216082329005</v>
+      </c>
+      <c r="T6">
+        <v>0.27735626906034</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="O7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="O8" t="s">
         <v>112</v>
       </c>
-      <c r="Q6">
+      <c r="Q8">
         <v>4418</v>
       </c>
-      <c r="R6">
+      <c r="R8">
         <v>489.85</v>
       </c>
-      <c r="S6">
+      <c r="S8">
         <v>786.935533612276</v>
       </c>
-      <c r="T6">
+      <c r="T8">
         <v>0.34911580938887699</v>
       </c>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34">
         <v>4418</v>
@@ -7413,10 +7524,10 @@
     </row>
     <row r="35" spans="2:7">
       <c r="B35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35">
         <v>697</v>
@@ -7433,10 +7544,10 @@
     </row>
     <row r="36" spans="2:7">
       <c r="B36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36">
         <v>697</v>
@@ -7453,10 +7564,10 @@
     </row>
     <row r="37" spans="2:7">
       <c r="B37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37">
         <v>697</v>
@@ -7473,10 +7584,10 @@
     </row>
     <row r="38" spans="2:7">
       <c r="B38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38">
         <v>697</v>
@@ -7493,10 +7604,10 @@
     </row>
     <row r="39" spans="2:7">
       <c r="B39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D39">
         <v>697</v>
@@ -7513,10 +7624,10 @@
     </row>
     <row r="40" spans="2:7">
       <c r="B40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40">
         <v>697</v>
@@ -7533,10 +7644,10 @@
     </row>
     <row r="41" spans="2:7">
       <c r="B41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D41">
         <v>697</v>
@@ -7553,10 +7664,10 @@
     </row>
     <row r="42" spans="2:7">
       <c r="B42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D42">
         <v>697</v>
@@ -7573,10 +7684,10 @@
     </row>
     <row r="43" spans="2:7">
       <c r="B43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D43">
         <v>697</v>
@@ -7593,10 +7704,10 @@
     </row>
     <row r="44" spans="2:7">
       <c r="B44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44">
         <v>697</v>
@@ -7613,10 +7724,10 @@
     </row>
     <row r="45" spans="2:7">
       <c r="B45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D45">
         <v>4418</v>
@@ -7633,10 +7744,10 @@
     </row>
     <row r="46" spans="2:7">
       <c r="B46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D46">
         <v>697</v>
@@ -7653,10 +7764,10 @@
     </row>
     <row r="47" spans="2:7">
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D47">
         <v>697</v>
@@ -7673,10 +7784,10 @@
     </row>
     <row r="48" spans="2:7">
       <c r="B48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D48">
         <v>4418</v>
@@ -7693,10 +7804,10 @@
     </row>
     <row r="49" spans="2:7">
       <c r="B49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D49">
         <v>697</v>
@@ -7713,10 +7824,10 @@
     </row>
     <row r="50" spans="2:7">
       <c r="B50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D50">
         <v>697</v>
@@ -7733,10 +7844,10 @@
     </row>
     <row r="51" spans="2:7">
       <c r="B51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D51">
         <v>697</v>
@@ -7753,10 +7864,10 @@
     </row>
     <row r="52" spans="2:7">
       <c r="B52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D52">
         <v>4418</v>
@@ -7773,10 +7884,10 @@
     </row>
     <row r="53" spans="2:7">
       <c r="B53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D53">
         <v>697</v>
@@ -7793,10 +7904,10 @@
     </row>
     <row r="54" spans="2:7">
       <c r="B54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D54">
         <v>697</v>
@@ -7813,10 +7924,10 @@
     </row>
     <row r="55" spans="2:7">
       <c r="B55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D55">
         <v>697</v>
@@ -7833,10 +7944,10 @@
     </row>
     <row r="56" spans="2:7">
       <c r="B56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D56">
         <v>697</v>
@@ -7853,10 +7964,10 @@
     </row>
     <row r="57" spans="2:7">
       <c r="B57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D57">
         <v>697</v>
@@ -7873,10 +7984,10 @@
     </row>
     <row r="58" spans="2:7">
       <c r="B58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D58">
         <v>4418</v>
@@ -7893,10 +8004,10 @@
     </row>
     <row r="59" spans="2:7">
       <c r="B59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D59">
         <v>697</v>
@@ -7913,10 +8024,10 @@
     </row>
     <row r="60" spans="2:7">
       <c r="B60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D60">
         <v>697</v>
@@ -7933,10 +8044,10 @@
     </row>
     <row r="61" spans="2:7">
       <c r="B61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D61">
         <v>697</v>
@@ -7953,10 +8064,10 @@
     </row>
     <row r="62" spans="2:7">
       <c r="B62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D62">
         <v>697</v>
@@ -7973,10 +8084,10 @@
     </row>
     <row r="63" spans="2:7">
       <c r="B63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D63">
         <v>697</v>
@@ -7993,10 +8104,10 @@
     </row>
     <row r="64" spans="2:7">
       <c r="B64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D64">
         <v>697</v>
@@ -8013,10 +8124,10 @@
     </row>
     <row r="65" spans="2:7">
       <c r="B65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D65">
         <v>697</v>
@@ -8033,10 +8144,10 @@
     </row>
     <row r="66" spans="2:7">
       <c r="B66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D66">
         <v>4418</v>
@@ -8053,10 +8164,10 @@
     </row>
     <row r="67" spans="2:7">
       <c r="B67" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D67">
         <v>697</v>
@@ -8073,10 +8184,10 @@
     </row>
     <row r="68" spans="2:7">
       <c r="B68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D68">
         <v>4418</v>
@@ -8093,10 +8204,10 @@
     </row>
     <row r="69" spans="2:7">
       <c r="B69" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C69" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D69">
         <v>697</v>
@@ -8113,10 +8224,10 @@
     </row>
     <row r="70" spans="2:7">
       <c r="B70" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D70">
         <v>697</v>
@@ -8133,10 +8244,10 @@
     </row>
     <row r="71" spans="2:7">
       <c r="B71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D71">
         <v>697</v>
@@ -8180,7 +8291,7 @@
     <row r="2" spans="1:35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1">
         <v>3416</v>
@@ -8199,7 +8310,7 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="1">
         <v>3636</v>
@@ -8218,7 +8329,7 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q2" s="1">
         <v>3719</v>
@@ -8237,7 +8348,7 @@
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X2" s="1">
         <v>3741</v>
@@ -8256,7 +8367,7 @@
       </c>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AE2" s="1">
         <v>3762</v>
@@ -8276,24 +8387,24 @@
     </row>
     <row r="3" spans="1:35">
       <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" t="s">
+      <c r="R3" t="s">
         <v>36</v>
       </c>
-      <c r="R3" t="s">
+      <c r="Y3" t="s">
         <v>37</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AF3" t="s">
         <v>38</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>1171</v>
@@ -8311,7 +8422,7 @@
         <v>11859.855330136401</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4">
         <v>1225</v>
@@ -8329,7 +8440,7 @@
         <v>6201.9711732639398</v>
       </c>
       <c r="P4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q4">
         <v>1252</v>
@@ -8347,7 +8458,7 @@
         <v>5289.6022753607704</v>
       </c>
       <c r="W4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X4">
         <v>1260</v>
@@ -8365,7 +8476,7 @@
         <v>878.58458178384899</v>
       </c>
       <c r="AD4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AE4">
         <v>1268</v>
@@ -8385,7 +8496,7 @@
     </row>
     <row r="5" spans="1:35">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>4265</v>
@@ -8403,7 +8514,7 @@
         <v>6146.8739335056098</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5">
         <v>4265</v>
@@ -8421,7 +8532,7 @@
         <v>2439.4270167761001</v>
       </c>
       <c r="P5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q5">
         <v>4265</v>
@@ -8439,7 +8550,7 @@
         <v>1638.6189707383401</v>
       </c>
       <c r="W5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X5">
         <v>4265</v>
@@ -8457,7 +8568,7 @@
         <v>291.52680657542197</v>
       </c>
       <c r="AD5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AE5">
         <v>4265</v>
@@ -8477,7 +8588,7 @@
     </row>
     <row r="6" spans="1:35">
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6">
         <v>221</v>
@@ -8495,7 +8606,7 @@
         <v>5685.7883881938797</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6">
         <v>287</v>
@@ -8513,7 +8624,7 @@
         <v>2140.0590929953801</v>
       </c>
       <c r="P6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q6">
         <v>328</v>
@@ -8531,7 +8642,7 @@
         <v>1345.79345830015</v>
       </c>
       <c r="W6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X6">
         <v>337</v>
@@ -8549,7 +8660,7 @@
         <v>252.32218606597999</v>
       </c>
       <c r="AD6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE6">
         <v>346</v>
@@ -8569,7 +8680,7 @@
     </row>
     <row r="7" spans="1:35">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>184</v>
@@ -8587,7 +8698,7 @@
         <v>5672.1373278576502</v>
       </c>
       <c r="I7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7">
         <v>184</v>
@@ -8605,7 +8716,7 @@
         <v>2120.6273310420502</v>
       </c>
       <c r="P7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q7">
         <v>184</v>
@@ -8623,7 +8734,7 @@
         <v>979.27852616543896</v>
       </c>
       <c r="W7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X7">
         <v>184</v>
@@ -8641,7 +8752,7 @@
         <v>228.494655351375</v>
       </c>
       <c r="AD7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AE7">
         <v>184</v>
@@ -8661,7 +8772,7 @@
     </row>
     <row r="8" spans="1:35">
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>18</v>
@@ -8679,7 +8790,7 @@
         <v>5552.3544902354397</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J8">
         <v>18</v>
@@ -8697,7 +8808,7 @@
         <v>2081.2161639765</v>
       </c>
       <c r="P8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q8">
         <v>18</v>
@@ -8715,7 +8826,7 @@
         <v>1056.5895793473901</v>
       </c>
       <c r="W8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X8">
         <v>18</v>
@@ -8733,7 +8844,7 @@
         <v>260.33175331305699</v>
       </c>
       <c r="AD8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AE8">
         <v>18</v>
@@ -8753,12 +8864,12 @@
     </row>
     <row r="12" spans="1:35">
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:35">
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13">
         <v>10193.3824</v>
@@ -8766,7 +8877,7 @@
     </row>
     <row r="14" spans="1:35">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>5539.2927</v>
@@ -8774,7 +8885,7 @@
     </row>
     <row r="15" spans="1:35">
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>5303.5681999999997</v>
@@ -8782,7 +8893,7 @@
     </row>
     <row r="16" spans="1:35">
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16">
         <v>5287.3666999999996</v>
@@ -8790,7 +8901,7 @@
     </row>
     <row r="17" spans="2:9">
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17">
         <v>5153.8462</v>
@@ -8798,15 +8909,15 @@
     </row>
     <row r="30" spans="2:9">
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31">
         <v>3805</v>
@@ -8830,7 +8941,7 @@
     </row>
     <row r="32" spans="2:9">
       <c r="B32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32">
         <v>1282</v>
@@ -8854,7 +8965,7 @@
     </row>
     <row r="33" spans="2:9">
       <c r="B33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33">
         <v>4265</v>
@@ -8878,7 +8989,7 @@
     </row>
     <row r="34" spans="2:9">
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>364</v>
@@ -8902,7 +9013,7 @@
     </row>
     <row r="35" spans="2:9">
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35">
         <v>184</v>
@@ -8926,7 +9037,7 @@
     </row>
     <row r="36" spans="2:9">
       <c r="B36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36">
         <v>18</v>
@@ -8946,7 +9057,7 @@
     </row>
     <row r="47" spans="2:9">
       <c r="I47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="2:9">
@@ -9006,27 +9117,27 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" t="s">
+      <c r="R1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" t="s">
         <v>50</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Z1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" t="s">
         <v>52</v>
-      </c>
-      <c r="U1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>3654</v>
@@ -9051,7 +9162,7 @@
         <v>164.97139999999999</v>
       </c>
       <c r="S2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T2">
         <v>3654</v>
@@ -9072,7 +9183,7 @@
         <v>291.47390000000001</v>
       </c>
       <c r="AA2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AB2">
         <v>3654</v>
@@ -9092,7 +9203,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>541</v>
@@ -9117,7 +9228,7 @@
         <v>120.2688</v>
       </c>
       <c r="S3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T3">
         <v>541</v>
@@ -9138,7 +9249,7 @@
         <v>251.53710000000001</v>
       </c>
       <c r="AA3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB3">
         <v>541</v>
@@ -9167,7 +9278,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -9175,7 +9286,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -9202,10 +9313,10 @@
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:16">
@@ -9213,7 +9324,7 @@
         <v>0.05</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>3994</v>
@@ -9231,7 +9342,7 @@
         <v>168.39603274311301</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L3">
         <v>13</v>
@@ -9254,7 +9365,7 @@
         <v>0.1</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4">
         <v>4355</v>
@@ -9272,7 +9383,7 @@
         <v>168.43765748429001</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L4">
         <v>4121</v>
@@ -9295,7 +9406,7 @@
         <v>0.25</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>4265</v>
@@ -9313,7 +9424,7 @@
         <v>164.99423393662599</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L5">
         <v>4355</v>
@@ -9336,7 +9447,7 @@
         <v>0.5</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6">
         <v>4368</v>
@@ -9354,7 +9465,7 @@
         <v>147.92409587328299</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L6">
         <v>4265</v>
@@ -9377,7 +9488,7 @@
         <v>0.75</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>4366</v>
@@ -9395,7 +9506,7 @@
         <v>111.48480722206899</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L7">
         <v>4368</v>
@@ -9418,7 +9529,7 @@
         <v>0.9</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>4340</v>
@@ -9436,7 +9547,7 @@
         <v>67.271245778883895</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L8">
         <v>4366</v>
@@ -9459,7 +9570,7 @@
         <v>0.95</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>3986</v>
@@ -9477,7 +9588,7 @@
         <v>41.595746391112598</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L9">
         <v>4113</v>
@@ -9497,7 +9608,7 @@
     </row>
     <row r="10" spans="2:16">
       <c r="K10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L10">
         <v>20</v>
@@ -9517,7 +9628,7 @@
     </row>
     <row r="11" spans="2:16">
       <c r="K11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L11">
         <v>22</v>
@@ -9537,7 +9648,7 @@
     </row>
     <row r="12" spans="2:16">
       <c r="K12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L12">
         <v>4340</v>
@@ -9579,7 +9690,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -9639,7 +9750,7 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -11277,43 +11388,43 @@
   <sheetData>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" t="s">
         <v>90</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>91</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>92</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="U4" t="s">
         <v>93</v>
-      </c>
-      <c r="U4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>2788</v>
@@ -11328,7 +11439,7 @@
         <v>0.87500761976709396</v>
       </c>
       <c r="I5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J5">
         <v>2788</v>
@@ -11343,7 +11454,7 @@
         <v>4.4534870113327001</v>
       </c>
       <c r="O5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P5">
         <v>2788</v>
@@ -11364,10 +11475,10 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <v>697</v>
@@ -11382,7 +11493,7 @@
         <v>2.1774689791695301</v>
       </c>
       <c r="I6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J6">
         <v>697</v>
@@ -11397,7 +11508,7 @@
         <v>0.70287368834331299</v>
       </c>
       <c r="O6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P6">
         <v>697</v>
@@ -11418,10 +11529,10 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7">
         <v>88</v>
@@ -11436,7 +11547,7 @@
         <v>91.185604585222904</v>
       </c>
       <c r="I7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J7">
         <v>88</v>
@@ -11451,7 +11562,7 @@
         <v>3.8532873209707099</v>
       </c>
       <c r="O7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P7">
         <v>88</v>
@@ -11472,10 +11583,10 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -11490,7 +11601,7 @@
         <v>468.412819286949</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J8">
         <v>30</v>
@@ -11505,7 +11616,7 @@
         <v>5.1971971990608496</v>
       </c>
       <c r="O8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P8">
         <v>30</v>
@@ -11526,10 +11637,10 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9">
         <v>26</v>
@@ -11544,7 +11655,7 @@
         <v>8729.2909631326202</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J9">
         <v>26</v>
@@ -11559,7 +11670,7 @@
         <v>2.9903048145519602</v>
       </c>
       <c r="O9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P9">
         <v>26</v>
@@ -11605,27 +11716,27 @@
   <sheetData>
     <row r="1" spans="2:31">
       <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>101</v>
       </c>
-      <c r="N1" t="s">
-        <v>102</v>
-      </c>
       <c r="S1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X1" t="s">
         <v>104</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AC1" t="s">
         <v>105</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="2:31">
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2">
         <v>5493</v>
@@ -11640,7 +11751,7 @@
         <v>9.0660788072870493E-2</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2">
         <v>5493</v>
@@ -11655,7 +11766,7 @@
         <v>8.6480739509190399E-2</v>
       </c>
       <c r="L2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M2">
         <v>5493</v>
@@ -11670,7 +11781,7 @@
         <v>5.37763105519561E-2</v>
       </c>
       <c r="Q2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R2">
         <v>5493</v>
@@ -11685,7 +11796,7 @@
         <v>6.0647182095143602E-2</v>
       </c>
       <c r="V2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W2">
         <v>5493</v>
@@ -11700,7 +11811,7 @@
         <v>3.5276286917571E-5</v>
       </c>
       <c r="AA2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AB2">
         <v>5493</v>
@@ -11717,7 +11828,7 @@
     </row>
     <row r="3" spans="2:31">
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3">
         <v>5494</v>
@@ -11732,7 +11843,7 @@
         <v>9.0643281831517597E-2</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3">
         <v>5494</v>
@@ -11747,7 +11858,7 @@
         <v>8.6463884836398094E-2</v>
       </c>
       <c r="L3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M3">
         <v>5494</v>
@@ -11762,7 +11873,7 @@
         <v>5.4936057568734903E-2</v>
       </c>
       <c r="Q3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R3">
         <v>5494</v>
@@ -11777,7 +11888,7 @@
         <v>6.1087659756118198E-2</v>
       </c>
       <c r="V3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W3">
         <v>5494</v>
@@ -11792,7 +11903,7 @@
         <v>2.7060472417163398E-4</v>
       </c>
       <c r="AA3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AB3">
         <v>5494</v>
@@ -11809,7 +11920,7 @@
     </row>
     <row r="4" spans="2:31">
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4">
         <v>5497</v>
@@ -11824,7 +11935,7 @@
         <v>9.0590238488394106E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H4">
         <v>5497</v>
@@ -11839,7 +11950,7 @@
         <v>8.6412863831662801E-2</v>
       </c>
       <c r="L4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M4">
         <v>5497</v>
@@ -11854,7 +11965,7 @@
         <v>5.9015454219437102E-2</v>
       </c>
       <c r="Q4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R4">
         <v>5497</v>
@@ -11869,7 +11980,7 @@
         <v>6.40072217753508E-2</v>
       </c>
       <c r="V4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="W4">
         <v>5497</v>
@@ -11884,7 +11995,7 @@
         <v>1.2530401635196899E-3</v>
       </c>
       <c r="AA4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AB4">
         <v>5497</v>
@@ -11901,7 +12012,7 @@
     </row>
     <row r="5" spans="2:31">
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5">
         <v>5499</v>
@@ -11916,7 +12027,7 @@
         <v>9.0550721174100998E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5">
         <v>5499</v>
@@ -11931,7 +12042,7 @@
         <v>8.6375988665648704E-2</v>
       </c>
       <c r="L5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M5">
         <v>5499</v>
@@ -11946,7 +12057,7 @@
         <v>6.4162376924033704E-2</v>
       </c>
       <c r="Q5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R5">
         <v>5499</v>
@@ -11961,7 +12072,7 @@
         <v>7.3094059343264101E-2</v>
       </c>
       <c r="V5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="W5">
         <v>5499</v>
@@ -11976,7 +12087,7 @@
         <v>2.17302766911914E-3</v>
       </c>
       <c r="AA5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB5">
         <v>5499</v>
@@ -11993,7 +12104,7 @@
     </row>
     <row r="6" spans="2:31">
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6">
         <v>5501</v>
@@ -12008,7 +12119,7 @@
         <v>9.0507465978203194E-2</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6">
         <v>5501</v>
@@ -12023,7 +12134,7 @@
         <v>8.6335322657928495E-2</v>
       </c>
       <c r="L6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M6">
         <v>5501</v>
@@ -12038,7 +12149,7 @@
         <v>7.1296533036076207E-2</v>
       </c>
       <c r="Q6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R6">
         <v>5501</v>
@@ -12053,7 +12164,7 @@
         <v>9.1585406147622797E-2</v>
       </c>
       <c r="V6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W6">
         <v>5501</v>
@@ -12068,7 +12179,7 @@
         <v>2.9684809627319102E-3</v>
       </c>
       <c r="AA6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB6">
         <v>5501</v>

</xml_diff>

<commit_message>
strong closed section done
</commit_message>
<xml_diff>
--- a/write-ups/cikm/performance.xlsx
+++ b/write-ups/cikm/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16560" tabRatio="500" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Change with Epochlength" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Buffer Size" sheetId="6" r:id="rId6"/>
     <sheet name="Maximal Itemsets" sheetId="7" r:id="rId7"/>
     <sheet name="len2+ " sheetId="8" r:id="rId8"/>
+    <sheet name="jaccard+May5th" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="169">
   <si>
     <t>MinSupp</t>
   </si>
@@ -408,6 +409,137 @@
   <si>
     <t>Maximal Itemsets</t>
   </si>
+  <si>
+    <t>select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'CPUMillisFilter' group by args order by args;</t>
+  </si>
+  <si>
+    <t>Runtime:</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.05_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.05]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.1_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.1]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.2_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.2]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.3_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.3]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.4_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.4]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.5_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.5]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.6_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.6]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.7_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.7]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.8_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.8]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.95_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.95]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_conf0.9_Buff1000,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.9]</t>
+  </si>
+  <si>
+    <t>Mean millis for filtering</t>
+  </si>
+  <si>
+    <t>AlliedLowConf:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'AlliedLowConf' group by args order by args;
+</t>
+  </si>
+  <si>
+    <t>ClosedItemsets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'EnoughCharsItemsets' group by args order by args;
+</t>
+  </si>
+  <si>
+    <t>StrongClosed</t>
+  </si>
+  <si>
+    <t>select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'StrongClosedIS' group by args order by args;</t>
+  </si>
+  <si>
+    <t>Over Confident:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'OverConfident' group by args order by args;
+</t>
+  </si>
+  <si>
+    <t>HighConfidence</t>
+  </si>
+  <si>
+    <t>select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'HighConfidenceIS' group by args order by args;</t>
+  </si>
+  <si>
+    <t>PercentStrongInConfident</t>
+  </si>
+  <si>
+    <t>Strong Closed</t>
+  </si>
+  <si>
+    <t>High Confidence</t>
+  </si>
+  <si>
+    <t>Len1 Itemsets:</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.05,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.05]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.1,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.1]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.2,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.2]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.3,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.3]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.4,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.4]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.5,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.5]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.6,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.6]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.7,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.7]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.8,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.8]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.95,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.95]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, NFLKld_Jaccard+_ULBuff_conf0.9,  ITEMSET_SIMILARITY_JACCARD_GOOD_THRESHOLD=0.8 ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=ITEMSET_SIMILARITY_BAD_THRESHOLD ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.9]</t>
+  </si>
+  <si>
+    <t>ULBuff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'Len1Itemsets' group by args order by args;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'Len2+Itemsets' group by args order by args;
+</t>
+  </si>
 </sst>
 </file>
 
@@ -468,7 +600,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="243">
+  <cellStyleXfs count="287">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -712,14 +844,61 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="243">
+  <cellStyles count="287">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -841,6 +1020,28 @@
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -962,6 +1163,28 @@
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2911,6 +3134,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3002,6 +3226,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3286,6 +3511,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3431,6 +3657,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3651,6 +3878,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3751,12 +3979,1252 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean millis for filtering</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$D$5:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1439.11137162954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1476.52989449004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1436.57913247362</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1492.11254396249</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1438.88862837046</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1409.16803374736</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1475.92731535756</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1412.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1410.59320046893</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1405.72567409144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1451.76553341149</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2119106104"/>
+        <c:axId val="-2118888488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2119106104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2118888488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2118888488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2119106104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th'!$Q$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AlliedLowConf:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$A$5:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$S$5:$S$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0133645955451348</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.046189917936694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.160140679953107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.980539273153576</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.68300117233294</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.98101710803843</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.71090269636577</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.9465416178195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.4370457209848</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.0281359906213</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17.5875732708089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th'!$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Over Confident:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$X$5:$X$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>66.4752637749121</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.1824150058617</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.8762016412661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.4480656506448</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58.010082063306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.0149988282165</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51.0794841735053</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.0686987104338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36.3856975381008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.8274325908558</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0145369284877</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2119027320"/>
+        <c:axId val="-2093449176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2119027320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2093449176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2093449176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2119027320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$N$5:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>207.322626025791</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.082063305979</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.504806565064</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>199.96694021102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191.577725674091</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>181.958509142053</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>169.097069167644</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>151.860726846424</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.602344665885</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.6841735052755</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.2888628370457</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$P$5:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>207.3092614302459</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.0358733880423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.3446658851109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198.9864009378664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.894724501758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.9774920340146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>161.3861664712782</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.9141852286045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110.1652989449002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.65603751465419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.7012895662368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2107929432"/>
+        <c:axId val="-2107854392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2107929432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2107854392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2107854392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2107929432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th'!$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strong Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$A$5:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$P$5:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>207.3092614302459</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.0358733880423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.3446658851109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198.9864009378664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.894724501758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.9774920340146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>161.3861664712782</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.9141852286045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110.1652989449002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.65603751465419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.7012895662368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2118905112"/>
+        <c:axId val="-2093942920"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2118905112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2093942920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2093942920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2118905112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th'!$AC$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HighConfidence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$AC$5:$AC$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>353.607268464244</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>353.337162954279</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>350.841266119578</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>340.07409144197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>323.465416178195</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>304.144363721584</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>279.018991793669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>248.754747948417</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>206.735756154748</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>127.873622508792</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70.2654161781946</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2095902568"/>
+        <c:axId val="-2108644776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2095902568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2108644776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2108644776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2095902568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th'!$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strong Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$A$5:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$P$5:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>207.3092614302459</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.0358733880423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.3446658851109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198.9864009378664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.894724501758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.9774920340146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>161.3861664712782</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.9141852286045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110.1652989449002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.65603751465419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.7012895662368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$Z$17:$Z$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.586269796802009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.585944234274707</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.585292226756253</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.585126611951329</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.583971933487001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.581886476107843</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.578405668495216</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.566478374345744</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.532879754300645</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.49780428727807</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.465396653786347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th'!$Z$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High Confidence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th'!$Z$5:$Z$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>146.2980070339981</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146.3012895662367</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145.4966002344671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>141.0876905041036</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>134.570691676437</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127.1668716875694</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>117.6328253223907</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>107.8405627198125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96.5704572098478</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.2175849941378</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37.5641266119578</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="95"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2093344584"/>
+        <c:axId val="-2090212792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2093344584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090212792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2090212792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2093344584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman"/>
+          <a:cs typeface="Times New Roman"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -6299,6 +7767,191 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6623,7 +8276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S976"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -13146,7 +14799,7 @@
   <dimension ref="A1:T71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13155,6 +14808,7 @@
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -14303,12 +15957,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="69" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15131,7 +16786,7 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z1" activeCellId="1" sqref="AC1:AC1048576 Z1:Z1048576"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17401,8 +19056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18226,4 +19881,1657 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AU39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AR5" sqref="AR5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:47" ht="285">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="L3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M3" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>141</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="V3" t="s">
+        <v>147</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>140</v>
+      </c>
+      <c r="P4" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47">
+      <c r="A5">
+        <v>0.05</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5">
+        <v>4265</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1439.1113716295399</v>
+      </c>
+      <c r="E5">
+        <v>407.23554710983802</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5">
+        <v>4265</v>
+      </c>
+      <c r="I5">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J5">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L5" t="s">
+        <v>129</v>
+      </c>
+      <c r="M5">
+        <v>4265</v>
+      </c>
+      <c r="N5">
+        <v>207.32262602579101</v>
+      </c>
+      <c r="O5">
+        <v>63.7310323226232</v>
+      </c>
+      <c r="P5">
+        <f>N5-S5</f>
+        <v>207.30926143024587</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>129</v>
+      </c>
+      <c r="R5">
+        <v>4265</v>
+      </c>
+      <c r="S5">
+        <v>1.33645955451348E-2</v>
+      </c>
+      <c r="T5">
+        <v>0.196258517611271</v>
+      </c>
+      <c r="V5" t="s">
+        <v>129</v>
+      </c>
+      <c r="W5">
+        <v>4265</v>
+      </c>
+      <c r="X5">
+        <v>66.475263774912094</v>
+      </c>
+      <c r="Y5">
+        <v>17.046190698738801</v>
+      </c>
+      <c r="Z5">
+        <f>AC5-P5</f>
+        <v>146.29800703399812</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB5">
+        <v>4265</v>
+      </c>
+      <c r="AC5">
+        <v>353.60726846424399</v>
+      </c>
+      <c r="AD5">
+        <v>129.23084190946</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN5">
+        <v>4265</v>
+      </c>
+      <c r="AO5">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP5">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AS5">
+        <v>4265</v>
+      </c>
+      <c r="AT5">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU5">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47">
+      <c r="A6">
+        <v>0.1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6">
+        <v>4265</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1476.5298944900401</v>
+      </c>
+      <c r="E6">
+        <v>405.60873184462503</v>
+      </c>
+      <c r="G6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6">
+        <v>4265</v>
+      </c>
+      <c r="I6">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J6">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L6" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6">
+        <v>4265</v>
+      </c>
+      <c r="N6">
+        <v>207.08206330597901</v>
+      </c>
+      <c r="O6">
+        <v>61.532106351598898</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P15" si="0">N6-S6</f>
+        <v>207.03587338804232</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6">
+        <v>4265</v>
+      </c>
+      <c r="S6">
+        <v>4.6189917936693997E-2</v>
+      </c>
+      <c r="T6">
+        <v>0.39458714090188002</v>
+      </c>
+      <c r="V6" t="s">
+        <v>130</v>
+      </c>
+      <c r="W6">
+        <v>4265</v>
+      </c>
+      <c r="X6">
+        <v>65.182415005861699</v>
+      </c>
+      <c r="Y6">
+        <v>16.769014026125799</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6:Z15" si="1">AC6-P6</f>
+        <v>146.30128956623668</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB6">
+        <v>4265</v>
+      </c>
+      <c r="AC6">
+        <v>353.33716295427899</v>
+      </c>
+      <c r="AD6">
+        <v>126.004469938871</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>130</v>
+      </c>
+      <c r="AN6">
+        <v>4265</v>
+      </c>
+      <c r="AO6">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP6">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS6">
+        <v>4265</v>
+      </c>
+      <c r="AT6">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU6">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47">
+      <c r="A7">
+        <v>0.2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7">
+        <v>4265</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1436.5791324736199</v>
+      </c>
+      <c r="E7">
+        <v>397.29148351794402</v>
+      </c>
+      <c r="G7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7">
+        <v>4265</v>
+      </c>
+      <c r="I7">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J7">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L7" t="s">
+        <v>131</v>
+      </c>
+      <c r="M7">
+        <v>4265</v>
+      </c>
+      <c r="N7">
+        <v>205.504806565064</v>
+      </c>
+      <c r="O7">
+        <v>54.759674823189201</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>205.34466588511089</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>131</v>
+      </c>
+      <c r="R7">
+        <v>4265</v>
+      </c>
+      <c r="S7">
+        <v>0.16014067995310699</v>
+      </c>
+      <c r="T7">
+        <v>1.1179945438560699</v>
+      </c>
+      <c r="V7" t="s">
+        <v>131</v>
+      </c>
+      <c r="W7">
+        <v>4265</v>
+      </c>
+      <c r="X7">
+        <v>62.8762016412661</v>
+      </c>
+      <c r="Y7">
+        <v>16.267685097752299</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="1"/>
+        <v>145.49660023446711</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB7">
+        <v>4265</v>
+      </c>
+      <c r="AC7">
+        <v>350.84126611957799</v>
+      </c>
+      <c r="AD7">
+        <v>118.90890329817501</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AN7">
+        <v>4265</v>
+      </c>
+      <c r="AO7">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP7">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AS7">
+        <v>4265</v>
+      </c>
+      <c r="AT7">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU7">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47">
+      <c r="A8">
+        <v>0.3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8">
+        <v>4265</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1492.11254396249</v>
+      </c>
+      <c r="E8">
+        <v>412.21364669353102</v>
+      </c>
+      <c r="G8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8">
+        <v>4265</v>
+      </c>
+      <c r="I8">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J8">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L8" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8">
+        <v>4265</v>
+      </c>
+      <c r="N8">
+        <v>199.96694021101999</v>
+      </c>
+      <c r="O8">
+        <v>48.833379503146702</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>198.98640093786642</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8">
+        <v>4265</v>
+      </c>
+      <c r="S8">
+        <v>0.98053927315357603</v>
+      </c>
+      <c r="T8">
+        <v>2.2896180953244301</v>
+      </c>
+      <c r="V8" t="s">
+        <v>132</v>
+      </c>
+      <c r="W8">
+        <v>4265</v>
+      </c>
+      <c r="X8">
+        <v>60.4480656506448</v>
+      </c>
+      <c r="Y8">
+        <v>15.7412737264897</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="1"/>
+        <v>141.08769050410356</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB8">
+        <v>4265</v>
+      </c>
+      <c r="AC8">
+        <v>340.07409144196998</v>
+      </c>
+      <c r="AD8">
+        <v>111.31241486203</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AN8">
+        <v>4265</v>
+      </c>
+      <c r="AO8">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP8">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS8">
+        <v>4265</v>
+      </c>
+      <c r="AT8">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU8">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47">
+      <c r="A9">
+        <v>0.4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9">
+        <v>4265</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1438.8886283704601</v>
+      </c>
+      <c r="E9">
+        <v>401.266794490655</v>
+      </c>
+      <c r="G9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9">
+        <v>4265</v>
+      </c>
+      <c r="I9">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J9">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L9" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9">
+        <v>4265</v>
+      </c>
+      <c r="N9">
+        <v>191.577725674091</v>
+      </c>
+      <c r="O9">
+        <v>42.661657246848897</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>188.89472450175805</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>133</v>
+      </c>
+      <c r="R9">
+        <v>4265</v>
+      </c>
+      <c r="S9">
+        <v>2.6830011723329399</v>
+      </c>
+      <c r="T9">
+        <v>3.9232020650241699</v>
+      </c>
+      <c r="V9" t="s">
+        <v>133</v>
+      </c>
+      <c r="W9">
+        <v>4265</v>
+      </c>
+      <c r="X9">
+        <v>58.010082063306001</v>
+      </c>
+      <c r="Y9">
+        <v>15.004162700003</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="1"/>
+        <v>134.57069167643698</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB9">
+        <v>4265</v>
+      </c>
+      <c r="AC9">
+        <v>323.46541617819503</v>
+      </c>
+      <c r="AD9">
+        <v>102.978630304823</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN9">
+        <v>4265</v>
+      </c>
+      <c r="AO9">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP9">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AS9">
+        <v>4265</v>
+      </c>
+      <c r="AT9">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU9">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47">
+      <c r="A10">
+        <v>0.5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10">
+        <v>4267</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1409.1680337473599</v>
+      </c>
+      <c r="E10">
+        <v>389.81734050599403</v>
+      </c>
+      <c r="G10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10">
+        <v>4267</v>
+      </c>
+      <c r="I10">
+        <v>6018.6184673072403</v>
+      </c>
+      <c r="J10">
+        <v>714.07086838665805</v>
+      </c>
+      <c r="L10" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10">
+        <v>4266</v>
+      </c>
+      <c r="N10">
+        <v>181.958509142053</v>
+      </c>
+      <c r="O10">
+        <v>39.511061137313398</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>176.97749203401457</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>134</v>
+      </c>
+      <c r="R10">
+        <v>4267</v>
+      </c>
+      <c r="S10">
+        <v>4.9810171080384302</v>
+      </c>
+      <c r="T10">
+        <v>6.2441245216712096</v>
+      </c>
+      <c r="V10" t="s">
+        <v>134</v>
+      </c>
+      <c r="W10">
+        <v>4267</v>
+      </c>
+      <c r="X10">
+        <v>55.014998828216498</v>
+      </c>
+      <c r="Y10">
+        <v>14.3594522113283</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="1"/>
+        <v>127.16687168756943</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB10">
+        <v>4267</v>
+      </c>
+      <c r="AC10">
+        <v>304.144363721584</v>
+      </c>
+      <c r="AD10">
+        <v>95.3965802219209</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AN10">
+        <v>4267</v>
+      </c>
+      <c r="AO10">
+        <v>3579.6904148113399</v>
+      </c>
+      <c r="AP10">
+        <v>304.97421825734699</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS10">
+        <v>4267</v>
+      </c>
+      <c r="AT10">
+        <v>2438.9280524958999</v>
+      </c>
+      <c r="AU10">
+        <v>569.48843744415694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47">
+      <c r="A11">
+        <v>0.6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11">
+        <v>4265</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1475.92731535756</v>
+      </c>
+      <c r="E11">
+        <v>410.642987972811</v>
+      </c>
+      <c r="G11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11">
+        <v>4265</v>
+      </c>
+      <c r="I11">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J11">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L11" t="s">
+        <v>135</v>
+      </c>
+      <c r="M11">
+        <v>4265</v>
+      </c>
+      <c r="N11">
+        <v>169.09706916764401</v>
+      </c>
+      <c r="O11">
+        <v>35.671295544680902</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>161.38616647127824</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>135</v>
+      </c>
+      <c r="R11">
+        <v>4265</v>
+      </c>
+      <c r="S11">
+        <v>7.7109026963657703</v>
+      </c>
+      <c r="T11">
+        <v>9.2423659363530106</v>
+      </c>
+      <c r="V11" t="s">
+        <v>135</v>
+      </c>
+      <c r="W11">
+        <v>4265</v>
+      </c>
+      <c r="X11">
+        <v>51.0794841735053</v>
+      </c>
+      <c r="Y11">
+        <v>13.4891212409829</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="1"/>
+        <v>117.63282532239074</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB11">
+        <v>4265</v>
+      </c>
+      <c r="AC11">
+        <v>279.01899179366899</v>
+      </c>
+      <c r="AD11">
+        <v>85.9900124300854</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN11">
+        <v>4265</v>
+      </c>
+      <c r="AO11">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP11">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AS11">
+        <v>4265</v>
+      </c>
+      <c r="AT11">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU11">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47">
+      <c r="A12">
+        <v>0.7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12">
+        <v>4265</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1412</v>
+      </c>
+      <c r="E12">
+        <v>382.66838621531099</v>
+      </c>
+      <c r="G12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12">
+        <v>4265</v>
+      </c>
+      <c r="I12">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J12">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L12" t="s">
+        <v>136</v>
+      </c>
+      <c r="M12">
+        <v>4265</v>
+      </c>
+      <c r="N12">
+        <v>151.860726846424</v>
+      </c>
+      <c r="O12">
+        <v>32.397968254699997</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>140.91418522860451</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>136</v>
+      </c>
+      <c r="R12">
+        <v>4265</v>
+      </c>
+      <c r="S12">
+        <v>10.9465416178195</v>
+      </c>
+      <c r="T12">
+        <v>12.673928894139801</v>
+      </c>
+      <c r="V12" t="s">
+        <v>136</v>
+      </c>
+      <c r="W12">
+        <v>4265</v>
+      </c>
+      <c r="X12">
+        <v>46.0686987104338</v>
+      </c>
+      <c r="Y12">
+        <v>12.475575305080699</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="1"/>
+        <v>107.84056271981248</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB12">
+        <v>4265</v>
+      </c>
+      <c r="AC12">
+        <v>248.75474794841699</v>
+      </c>
+      <c r="AD12">
+        <v>76.109555963721505</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN12">
+        <v>4265</v>
+      </c>
+      <c r="AO12">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP12">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AS12">
+        <v>4265</v>
+      </c>
+      <c r="AT12">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU12">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47">
+      <c r="A13">
+        <v>0.8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13">
+        <v>4265</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1410.59320046893</v>
+      </c>
+      <c r="E13">
+        <v>381.71928847997401</v>
+      </c>
+      <c r="G13" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13">
+        <v>4265</v>
+      </c>
+      <c r="I13">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J13">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L13" t="s">
+        <v>137</v>
+      </c>
+      <c r="M13">
+        <v>4265</v>
+      </c>
+      <c r="N13">
+        <v>124.602344665885</v>
+      </c>
+      <c r="O13">
+        <v>26.664449460758501</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>110.1652989449002</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>137</v>
+      </c>
+      <c r="R13">
+        <v>4265</v>
+      </c>
+      <c r="S13">
+        <v>14.4370457209848</v>
+      </c>
+      <c r="T13">
+        <v>11.954252883467699</v>
+      </c>
+      <c r="V13" t="s">
+        <v>137</v>
+      </c>
+      <c r="W13">
+        <v>4265</v>
+      </c>
+      <c r="X13">
+        <v>36.3856975381008</v>
+      </c>
+      <c r="Y13">
+        <v>10.6022729291426</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="1"/>
+        <v>96.570457209847802</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB13">
+        <v>4265</v>
+      </c>
+      <c r="AC13">
+        <v>206.735756154748</v>
+      </c>
+      <c r="AD13">
+        <v>66.313576519894099</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN13">
+        <v>4265</v>
+      </c>
+      <c r="AO13">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP13">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS13">
+        <v>4265</v>
+      </c>
+      <c r="AT13">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU13">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47">
+      <c r="A14">
+        <v>0.9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14">
+        <v>4265</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1405.7256740914399</v>
+      </c>
+      <c r="E14">
+        <v>360.79180532744499</v>
+      </c>
+      <c r="G14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14">
+        <v>4265</v>
+      </c>
+      <c r="I14">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J14">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L14" t="s">
+        <v>139</v>
+      </c>
+      <c r="M14">
+        <v>4265</v>
+      </c>
+      <c r="N14">
+        <v>82.684173505275496</v>
+      </c>
+      <c r="O14">
+        <v>20.602359548738999</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>63.656037514654194</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R14">
+        <v>4265</v>
+      </c>
+      <c r="S14">
+        <v>19.028135990621301</v>
+      </c>
+      <c r="T14">
+        <v>11.3704529670408</v>
+      </c>
+      <c r="V14" t="s">
+        <v>139</v>
+      </c>
+      <c r="W14">
+        <v>4265</v>
+      </c>
+      <c r="X14">
+        <v>20.8274325908558</v>
+      </c>
+      <c r="Y14">
+        <v>6.8957152585864696</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="1"/>
+        <v>64.217584994137809</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB14">
+        <v>4265</v>
+      </c>
+      <c r="AC14">
+        <v>127.873622508792</v>
+      </c>
+      <c r="AD14">
+        <v>51.070052876235401</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN14">
+        <v>4265</v>
+      </c>
+      <c r="AO14">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP14">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS14">
+        <v>4265</v>
+      </c>
+      <c r="AT14">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU14">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47">
+      <c r="A15">
+        <v>0.95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15">
+        <v>4265</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1451.76553341149</v>
+      </c>
+      <c r="E15">
+        <v>370.12522776019199</v>
+      </c>
+      <c r="G15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15">
+        <v>4265</v>
+      </c>
+      <c r="I15">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J15">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L15" t="s">
+        <v>138</v>
+      </c>
+      <c r="M15">
+        <v>4265</v>
+      </c>
+      <c r="N15">
+        <v>50.288862837045698</v>
+      </c>
+      <c r="O15">
+        <v>18.362197336857601</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>32.701289566236795</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>138</v>
+      </c>
+      <c r="R15">
+        <v>4265</v>
+      </c>
+      <c r="S15">
+        <v>17.5875732708089</v>
+      </c>
+      <c r="T15">
+        <v>12.8278720546367</v>
+      </c>
+      <c r="V15" t="s">
+        <v>138</v>
+      </c>
+      <c r="W15">
+        <v>4265</v>
+      </c>
+      <c r="X15">
+        <v>12.014536928487701</v>
+      </c>
+      <c r="Y15">
+        <v>4.4792909639774896</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="1"/>
+        <v>37.564126611957803</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB15">
+        <v>4265</v>
+      </c>
+      <c r="AC15">
+        <v>70.265416178194599</v>
+      </c>
+      <c r="AD15">
+        <v>38.763485061705303</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN15">
+        <v>4265</v>
+      </c>
+      <c r="AO15">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP15">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>138</v>
+      </c>
+      <c r="AS15">
+        <v>4265</v>
+      </c>
+      <c r="AT15">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU15">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47">
+      <c r="Z16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="26:47">
+      <c r="Z17" s="3">
+        <f>P5/AC5</f>
+        <v>0.5862697968020093</v>
+      </c>
+    </row>
+    <row r="18" spans="26:47">
+      <c r="Z18" s="3">
+        <f t="shared" ref="Z18:Z24" si="2">P6/AC6</f>
+        <v>0.58594423427470688</v>
+      </c>
+    </row>
+    <row r="19" spans="26:47">
+      <c r="Z19" s="3">
+        <f t="shared" si="2"/>
+        <v>0.58529222675625281</v>
+      </c>
+    </row>
+    <row r="20" spans="26:47">
+      <c r="Z20" s="3">
+        <f t="shared" si="2"/>
+        <v>0.5851266119513292</v>
+      </c>
+    </row>
+    <row r="21" spans="26:47">
+      <c r="Z21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.58397193348700116</v>
+      </c>
+    </row>
+    <row r="22" spans="26:47">
+      <c r="Z22" s="3">
+        <f t="shared" si="2"/>
+        <v>0.58188647610784294</v>
+      </c>
+    </row>
+    <row r="23" spans="26:47">
+      <c r="Z23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.5784056684952158</v>
+      </c>
+    </row>
+    <row r="24" spans="26:47">
+      <c r="Z24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.56647837434574377</v>
+      </c>
+    </row>
+    <row r="25" spans="26:47">
+      <c r="Z25" s="3">
+        <f>P13/AC13</f>
+        <v>0.53287975430064516</v>
+      </c>
+    </row>
+    <row r="26" spans="26:47">
+      <c r="Z26" s="3">
+        <f t="shared" ref="Z26:Z44" si="3">P14/AC14</f>
+        <v>0.49780428727807019</v>
+      </c>
+    </row>
+    <row r="27" spans="26:47">
+      <c r="Z27" s="3">
+        <f t="shared" si="3"/>
+        <v>0.4653966537863467</v>
+      </c>
+    </row>
+    <row r="28" spans="26:47">
+      <c r="AM28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="26:47">
+      <c r="AM29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN29" s="1">
+        <v>1464</v>
+      </c>
+      <c r="AO29" s="1">
+        <v>3600.1045079999999</v>
+      </c>
+      <c r="AP29" s="1">
+        <v>322.67472500000002</v>
+      </c>
+      <c r="AR29" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS29">
+        <v>1491</v>
+      </c>
+      <c r="AT29">
+        <v>2453.6277665995999</v>
+      </c>
+      <c r="AU29">
+        <v>549.89631750632998</v>
+      </c>
+    </row>
+    <row r="30" spans="26:47">
+      <c r="AM30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN30" s="1">
+        <v>1470</v>
+      </c>
+      <c r="AO30" s="1">
+        <v>3599.3224489999998</v>
+      </c>
+      <c r="AP30" s="1">
+        <v>322.32970990000001</v>
+      </c>
+      <c r="AR30" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS30">
+        <v>1501</v>
+      </c>
+      <c r="AT30">
+        <v>2452.04596935376</v>
+      </c>
+      <c r="AU30">
+        <v>548.76528426891502</v>
+      </c>
+    </row>
+    <row r="31" spans="26:47">
+      <c r="AM31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AN31" s="1">
+        <v>1472</v>
+      </c>
+      <c r="AO31" s="1">
+        <v>3599.3091030000001</v>
+      </c>
+      <c r="AP31" s="1">
+        <v>322.23685649999999</v>
+      </c>
+      <c r="AR31" t="s">
+        <v>157</v>
+      </c>
+      <c r="AS31">
+        <v>1503</v>
+      </c>
+      <c r="AT31">
+        <v>2452.1357285429099</v>
+      </c>
+      <c r="AU31">
+        <v>548.409477429356</v>
+      </c>
+    </row>
+    <row r="32" spans="26:47">
+      <c r="AM32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AN32" s="1">
+        <v>1477</v>
+      </c>
+      <c r="AO32" s="1">
+        <v>3600.6194989999999</v>
+      </c>
+      <c r="AP32" s="1">
+        <v>322.84104689999998</v>
+      </c>
+      <c r="AR32" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS32">
+        <v>1509</v>
+      </c>
+      <c r="AT32">
+        <v>2452.40490390987</v>
+      </c>
+      <c r="AU32">
+        <v>547.34953820989801</v>
+      </c>
+    </row>
+    <row r="33" spans="39:47">
+      <c r="AM33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AN33" s="1">
+        <v>1473</v>
+      </c>
+      <c r="AO33" s="1">
+        <v>3599.5736590000001</v>
+      </c>
+      <c r="AP33" s="1">
+        <v>322.2873649</v>
+      </c>
+      <c r="AR33" t="s">
+        <v>159</v>
+      </c>
+      <c r="AS33">
+        <v>1504</v>
+      </c>
+      <c r="AT33">
+        <v>2452.1728723404299</v>
+      </c>
+      <c r="AU33">
+        <v>548.22890126214895</v>
+      </c>
+    </row>
+    <row r="34" spans="39:47">
+      <c r="AM34" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN34" s="1">
+        <v>1470</v>
+      </c>
+      <c r="AO34" s="1">
+        <v>3599.3224489999998</v>
+      </c>
+      <c r="AP34" s="1">
+        <v>322.32970990000001</v>
+      </c>
+      <c r="AR34" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS34">
+        <v>1499</v>
+      </c>
+      <c r="AT34">
+        <v>2451.9666444296199</v>
+      </c>
+      <c r="AU34">
+        <v>549.12259322000295</v>
+      </c>
+    </row>
+    <row r="35" spans="39:47">
+      <c r="AM35" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AN35" s="1">
+        <v>1492</v>
+      </c>
+      <c r="AO35" s="1">
+        <v>3602.152145</v>
+      </c>
+      <c r="AP35" s="1">
+        <v>322.4974459</v>
+      </c>
+      <c r="AR35" t="s">
+        <v>161</v>
+      </c>
+      <c r="AS35">
+        <v>1518</v>
+      </c>
+      <c r="AT35">
+        <v>2453.2694334650901</v>
+      </c>
+      <c r="AU35">
+        <v>545.89095305868602</v>
+      </c>
+    </row>
+    <row r="36" spans="39:47">
+      <c r="AM36" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AN36" s="1">
+        <v>1480</v>
+      </c>
+      <c r="AO36" s="1">
+        <v>3601.528378</v>
+      </c>
+      <c r="AP36" s="1">
+        <v>323.1530333</v>
+      </c>
+      <c r="AR36" t="s">
+        <v>162</v>
+      </c>
+      <c r="AS36">
+        <v>1511</v>
+      </c>
+      <c r="AT36">
+        <v>2452.5512905360702</v>
+      </c>
+      <c r="AU36">
+        <v>547.00189823452604</v>
+      </c>
+    </row>
+    <row r="37" spans="39:47">
+      <c r="AM37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN37" s="1">
+        <v>1471</v>
+      </c>
+      <c r="AO37" s="1">
+        <v>3599.4819849999999</v>
+      </c>
+      <c r="AP37" s="1">
+        <v>322.2781463</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>163</v>
+      </c>
+      <c r="AS37">
+        <v>1501</v>
+      </c>
+      <c r="AT37">
+        <v>2452.04596935376</v>
+      </c>
+      <c r="AU37">
+        <v>548.76528426891502</v>
+      </c>
+    </row>
+    <row r="38" spans="39:47">
+      <c r="AM38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN38" s="1">
+        <v>1492</v>
+      </c>
+      <c r="AO38" s="1">
+        <v>3602.152145</v>
+      </c>
+      <c r="AP38" s="1">
+        <v>322.4974459</v>
+      </c>
+      <c r="AR38" t="s">
+        <v>164</v>
+      </c>
+      <c r="AS38">
+        <v>1519</v>
+      </c>
+      <c r="AT38">
+        <v>2453.5523370638598</v>
+      </c>
+      <c r="AU38">
+        <v>545.82249499294005</v>
+      </c>
+    </row>
+    <row r="39" spans="39:47">
+      <c r="AM39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AN39" s="1">
+        <v>1492</v>
+      </c>
+      <c r="AO39" s="1">
+        <v>3602.152145</v>
+      </c>
+      <c r="AP39" s="1">
+        <v>322.4974459</v>
+      </c>
+      <c r="AR39" t="s">
+        <v>165</v>
+      </c>
+      <c r="AS39">
+        <v>1518</v>
+      </c>
+      <c r="AT39">
+        <v>2453.2694334650901</v>
+      </c>
+      <c r="AU39">
+        <v>545.89095305868602</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tables for examples are beautified
</commit_message>
<xml_diff>
--- a/write-ups/cikm/performance.xlsx
+++ b/write-ups/cikm/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16560" tabRatio="500" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16560" tabRatio="500" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Change with Epochlength" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,8 @@
     <sheet name="Maximal Itemsets" sheetId="7" r:id="rId7"/>
     <sheet name="len2+ " sheetId="8" r:id="rId8"/>
     <sheet name="jaccard+May5th" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
+    <sheet name="jaccard+May5th (2)" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="179">
   <si>
     <t>MinSupp</t>
   </si>
@@ -540,6 +542,36 @@
     <t xml:space="preserve">select args, count(*), avg(value), stddev(value) from perf_mon where args like '%oct-nov-dec/%Jaccard+%' and key = 'Len2+Itemsets' group by args order by args;
 </t>
   </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.1_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.1]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.2_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.2]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.3_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.3]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.4_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.4]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.5_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.5]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.6_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.6]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.7_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.7]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.8_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.8]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.95_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.95]</t>
+  </si>
+  <si>
+    <t>[/home/yaboulna/fim_out/lcm_closed_cikm/4wk+1wk_ngram5-relsupp1_oct-nov-dec/, /home/yaboulna/fim_out/lcm_closed_cikm/1hr+30min_ngram5-relsupp10_oct-nov-dec/, Jaccard+NoCos_conf0.9_Buff1000,  ITEMSET_SIMILARITY_COSINE_GOOD_THRESHOLD=0.66 ITEMSET_SIMILARITY_PROMISING_THRESHOLD=0.0 ITEMSET_SIMILARITY_PPJOIN_MIN_LENGTH=3 ITEMSET_SIMILARITY_BAD_THRESHOLD=0.1 CONFIDENCE_HIGH_THRESHOLD=0.9]</t>
+  </si>
 </sst>
 </file>
 
@@ -600,8 +632,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="287">
+  <cellStyleXfs count="307">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -898,7 +950,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="287">
+  <cellStyles count="307">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1042,6 +1094,16 @@
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1185,6 +1247,16 @@
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5624,6 +5696,1229 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman"/>
+          <a:cs typeface="Times New Roman"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th (2)'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean millis for filtering</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$D$5:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1439.11137162954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1476.52989449004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1436.57913247362</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1492.11254396249</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1438.88862837046</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1409.16803374736</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1475.92731535756</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1412.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1410.59320046893</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1405.72567409144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1451.76553341149</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2092712536"/>
+        <c:axId val="-2092709528"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2092712536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2092709528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2092709528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2092712536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th (2)'!$Q$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AlliedLowConf:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$S$5:$S$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0133645955451348</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.046189917936694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.160140679953107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.980539273153576</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.68300117233294</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.98101710803843</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.71090269636577</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.9465416178195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.4370457209848</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.0281359906213</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17.5875732708089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th (2)'!$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Over Confident:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$X$5:$X$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>169.602674307545</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>170.025592417062</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170.409990574929</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>170.257416267943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>170.885924563017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171.581272084806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>172.618889809445</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>174.442166910688</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>179.521617069062</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>189.471601489758</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2091628136"/>
+        <c:axId val="-2090930696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2091628136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090930696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2090930696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2091628136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$N$5:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>207.322626025791</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.082063305979</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.504806565064</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>199.96694021102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191.577725674091</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>181.958509142053</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>169.097069167644</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>151.860726846424</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.602344665885</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.6841735052755</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.2888628370457</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$P$5:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>207.3092614302459</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.0358733880423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.3446658851109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198.9864009378664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.894724501758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.9774920340146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>161.3861664712782</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.9141852286045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110.1652989449002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.65603751465419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.7012895662368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2123898904"/>
+        <c:axId val="-2084655608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2123898904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2084655608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2084655608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2123898904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th (2)'!$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strong Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$P$5:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>207.3092614302459</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.0358733880423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.3446658851109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198.9864009378664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.894724501758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.9774920340146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>161.3861664712782</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.9141852286045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110.1652989449002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.65603751465419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.7012895662368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2094592184"/>
+        <c:axId val="-2093289064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2094592184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2093289064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2093289064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2094592184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th (2)'!$AC$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HighConfidence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$AC$5:$AC$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>361.0596285435</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>358.408560311284</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>343.21118611379</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>322.411937377691</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>297.063789868668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>264.723672367237</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230.757421543681</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>187.69843633656</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>113.837155963303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>62.0966206568301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2088149304"/>
+        <c:axId val="-2088415816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2088149304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2088415816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2088415816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2088149304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th (2)'!$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strong Closed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$P$5:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>207.3092614302459</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.0358733880423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.3446658851109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198.9864009378664</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.894724501758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.9774920340146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>161.3861664712782</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.9141852286045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110.1652989449002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.65603751465419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.7012895662368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$Z$17:$Z$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.574169043120448</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.577653260313392</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.598304117678233</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61718062475076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.635872600242758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.668536706413256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.699375844086249</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.750747784472391</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.774094914982833</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.559185065508617</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'jaccard+May5th (2)'!$Z$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High Confidence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'jaccard+May5th (2)'!$Z$5:$Z$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>153.7503671132542</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>151.3726869232417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>137.8665202286791</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>123.4255364398246</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>108.1690653669099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.74618033322241</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69.37125507240276</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.7842511079555</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-48.0686782880701</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.18111844864881</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="95"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2087918456"/>
+        <c:axId val="-2093466712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2087918456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2093466712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2093466712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2087918456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:txPr>
@@ -7952,6 +9247,203 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -14794,6 +16286,1649 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AU39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:47" ht="285">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="L3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M3" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>141</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="V3" t="s">
+        <v>147</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>140</v>
+      </c>
+      <c r="P4" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47">
+      <c r="A5">
+        <v>0.1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5">
+        <v>4265</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1439.1113716295399</v>
+      </c>
+      <c r="E5">
+        <v>407.23554710983802</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5">
+        <v>4265</v>
+      </c>
+      <c r="I5">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J5">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L5" t="s">
+        <v>129</v>
+      </c>
+      <c r="M5">
+        <v>4265</v>
+      </c>
+      <c r="N5">
+        <v>207.32262602579101</v>
+      </c>
+      <c r="O5">
+        <v>63.7310323226232</v>
+      </c>
+      <c r="P5">
+        <f>N5-S5</f>
+        <v>207.30926143024587</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>129</v>
+      </c>
+      <c r="R5">
+        <v>4265</v>
+      </c>
+      <c r="S5">
+        <v>1.33645955451348E-2</v>
+      </c>
+      <c r="T5">
+        <v>0.196258517611271</v>
+      </c>
+      <c r="V5" t="s">
+        <v>169</v>
+      </c>
+      <c r="W5">
+        <v>1047</v>
+      </c>
+      <c r="X5">
+        <v>169.60267430754499</v>
+      </c>
+      <c r="Y5">
+        <v>31.223561856728899</v>
+      </c>
+      <c r="Z5">
+        <f>AC5-P5</f>
+        <v>153.75036711325416</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB5">
+        <v>1023</v>
+      </c>
+      <c r="AC5">
+        <v>361.05962854350003</v>
+      </c>
+      <c r="AD5">
+        <v>148.57940270007501</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN5">
+        <v>4265</v>
+      </c>
+      <c r="AO5">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP5">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AS5">
+        <v>4265</v>
+      </c>
+      <c r="AT5">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU5">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47">
+      <c r="A6">
+        <v>0.2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6">
+        <v>4265</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1476.5298944900401</v>
+      </c>
+      <c r="E6">
+        <v>405.60873184462503</v>
+      </c>
+      <c r="G6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6">
+        <v>4265</v>
+      </c>
+      <c r="I6">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J6">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L6" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6">
+        <v>4265</v>
+      </c>
+      <c r="N6">
+        <v>207.08206330597901</v>
+      </c>
+      <c r="O6">
+        <v>61.532106351598898</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P15" si="0">N6-S6</f>
+        <v>207.03587338804232</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6">
+        <v>4265</v>
+      </c>
+      <c r="S6">
+        <v>4.6189917936693997E-2</v>
+      </c>
+      <c r="T6">
+        <v>0.39458714090188002</v>
+      </c>
+      <c r="V6" t="s">
+        <v>170</v>
+      </c>
+      <c r="W6">
+        <v>1055</v>
+      </c>
+      <c r="X6">
+        <v>170.025592417062</v>
+      </c>
+      <c r="Y6">
+        <v>31.174880247541001</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ref="Z6:Z14" si="1">AC6-P6</f>
+        <v>151.3726869232417</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB6">
+        <v>1028</v>
+      </c>
+      <c r="AC6">
+        <v>358.40856031128402</v>
+      </c>
+      <c r="AD6">
+        <v>146.52939330026501</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>130</v>
+      </c>
+      <c r="AN6">
+        <v>4265</v>
+      </c>
+      <c r="AO6">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP6">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS6">
+        <v>4265</v>
+      </c>
+      <c r="AT6">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU6">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47">
+      <c r="A7">
+        <v>0.3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7">
+        <v>4265</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1436.5791324736199</v>
+      </c>
+      <c r="E7">
+        <v>397.29148351794402</v>
+      </c>
+      <c r="G7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7">
+        <v>4265</v>
+      </c>
+      <c r="I7">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J7">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L7" t="s">
+        <v>131</v>
+      </c>
+      <c r="M7">
+        <v>4265</v>
+      </c>
+      <c r="N7">
+        <v>205.504806565064</v>
+      </c>
+      <c r="O7">
+        <v>54.759674823189201</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>205.34466588511089</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>131</v>
+      </c>
+      <c r="R7">
+        <v>4265</v>
+      </c>
+      <c r="S7">
+        <v>0.16014067995310699</v>
+      </c>
+      <c r="T7">
+        <v>1.1179945438560699</v>
+      </c>
+      <c r="V7" t="s">
+        <v>171</v>
+      </c>
+      <c r="W7">
+        <v>1061</v>
+      </c>
+      <c r="X7">
+        <v>170.409990574929</v>
+      </c>
+      <c r="Y7">
+        <v>31.0971189301297</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="1"/>
+        <v>137.86652022867912</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB7">
+        <v>1037</v>
+      </c>
+      <c r="AC7">
+        <v>343.21118611379001</v>
+      </c>
+      <c r="AD7">
+        <v>138.96451989557599</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AN7">
+        <v>4265</v>
+      </c>
+      <c r="AO7">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP7">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AS7">
+        <v>4265</v>
+      </c>
+      <c r="AT7">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU7">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47">
+      <c r="A8">
+        <v>0.4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8">
+        <v>4265</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1492.11254396249</v>
+      </c>
+      <c r="E8">
+        <v>412.21364669353102</v>
+      </c>
+      <c r="G8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8">
+        <v>4265</v>
+      </c>
+      <c r="I8">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J8">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L8" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8">
+        <v>4265</v>
+      </c>
+      <c r="N8">
+        <v>199.96694021101999</v>
+      </c>
+      <c r="O8">
+        <v>48.833379503146702</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>198.98640093786642</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8">
+        <v>4265</v>
+      </c>
+      <c r="S8">
+        <v>0.98053927315357603</v>
+      </c>
+      <c r="T8">
+        <v>2.2896180953244301</v>
+      </c>
+      <c r="V8" t="s">
+        <v>172</v>
+      </c>
+      <c r="W8">
+        <v>1045</v>
+      </c>
+      <c r="X8">
+        <v>170.257416267943</v>
+      </c>
+      <c r="Y8">
+        <v>31.172301952642901</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="1"/>
+        <v>123.42553643982458</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB8">
+        <v>1022</v>
+      </c>
+      <c r="AC8">
+        <v>322.411937377691</v>
+      </c>
+      <c r="AD8">
+        <v>129.74888567669001</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AN8">
+        <v>4265</v>
+      </c>
+      <c r="AO8">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP8">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS8">
+        <v>4265</v>
+      </c>
+      <c r="AT8">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU8">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9">
+        <v>4265</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1438.8886283704601</v>
+      </c>
+      <c r="E9">
+        <v>401.266794490655</v>
+      </c>
+      <c r="G9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9">
+        <v>4265</v>
+      </c>
+      <c r="I9">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J9">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L9" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9">
+        <v>4265</v>
+      </c>
+      <c r="N9">
+        <v>191.577725674091</v>
+      </c>
+      <c r="O9">
+        <v>42.661657246848897</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>188.89472450175805</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>133</v>
+      </c>
+      <c r="R9">
+        <v>4265</v>
+      </c>
+      <c r="S9">
+        <v>2.6830011723329399</v>
+      </c>
+      <c r="T9">
+        <v>3.9232020650241699</v>
+      </c>
+      <c r="V9" t="s">
+        <v>173</v>
+      </c>
+      <c r="W9">
+        <v>1087</v>
+      </c>
+      <c r="X9">
+        <v>170.885924563017</v>
+      </c>
+      <c r="Y9">
+        <v>31.263035655302701</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="1"/>
+        <v>108.16906536690993</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB9">
+        <v>1066</v>
+      </c>
+      <c r="AC9">
+        <v>297.06378986866798</v>
+      </c>
+      <c r="AD9">
+        <v>115.127990267329</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN9">
+        <v>4265</v>
+      </c>
+      <c r="AO9">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP9">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AS9">
+        <v>4265</v>
+      </c>
+      <c r="AT9">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU9">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47">
+      <c r="A10">
+        <v>0.6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10">
+        <v>4267</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1409.1680337473599</v>
+      </c>
+      <c r="E10">
+        <v>389.81734050599403</v>
+      </c>
+      <c r="G10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10">
+        <v>4267</v>
+      </c>
+      <c r="I10">
+        <v>6018.6184673072403</v>
+      </c>
+      <c r="J10">
+        <v>714.07086838665805</v>
+      </c>
+      <c r="L10" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10">
+        <v>4266</v>
+      </c>
+      <c r="N10">
+        <v>181.958509142053</v>
+      </c>
+      <c r="O10">
+        <v>39.511061137313398</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>176.97749203401457</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>134</v>
+      </c>
+      <c r="R10">
+        <v>4267</v>
+      </c>
+      <c r="S10">
+        <v>4.9810171080384302</v>
+      </c>
+      <c r="T10">
+        <v>6.2441245216712096</v>
+      </c>
+      <c r="V10" t="s">
+        <v>174</v>
+      </c>
+      <c r="W10">
+        <v>1132</v>
+      </c>
+      <c r="X10">
+        <v>171.58127208480599</v>
+      </c>
+      <c r="Y10">
+        <v>31.2175776700625</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="1"/>
+        <v>87.746180333222412</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB10">
+        <v>1111</v>
+      </c>
+      <c r="AC10">
+        <v>264.72367236723699</v>
+      </c>
+      <c r="AD10">
+        <v>95.878161081903897</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AN10">
+        <v>4267</v>
+      </c>
+      <c r="AO10">
+        <v>3579.6904148113399</v>
+      </c>
+      <c r="AP10">
+        <v>304.97421825734699</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS10">
+        <v>4267</v>
+      </c>
+      <c r="AT10">
+        <v>2438.9280524958999</v>
+      </c>
+      <c r="AU10">
+        <v>569.48843744415694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47">
+      <c r="A11">
+        <v>0.7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11">
+        <v>4265</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1475.92731535756</v>
+      </c>
+      <c r="E11">
+        <v>410.642987972811</v>
+      </c>
+      <c r="G11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11">
+        <v>4265</v>
+      </c>
+      <c r="I11">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J11">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L11" t="s">
+        <v>135</v>
+      </c>
+      <c r="M11">
+        <v>4265</v>
+      </c>
+      <c r="N11">
+        <v>169.09706916764401</v>
+      </c>
+      <c r="O11">
+        <v>35.671295544680902</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>161.38616647127824</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>135</v>
+      </c>
+      <c r="R11">
+        <v>4265</v>
+      </c>
+      <c r="S11">
+        <v>7.7109026963657703</v>
+      </c>
+      <c r="T11">
+        <v>9.2423659363530106</v>
+      </c>
+      <c r="V11" t="s">
+        <v>175</v>
+      </c>
+      <c r="W11">
+        <v>1207</v>
+      </c>
+      <c r="X11">
+        <v>172.61888980944499</v>
+      </c>
+      <c r="Y11">
+        <v>31.191681095751498</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="1"/>
+        <v>69.371255072402761</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB11">
+        <v>1179</v>
+      </c>
+      <c r="AC11">
+        <v>230.75742154368101</v>
+      </c>
+      <c r="AD11">
+        <v>73.299561088895302</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN11">
+        <v>4265</v>
+      </c>
+      <c r="AO11">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP11">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AS11">
+        <v>4265</v>
+      </c>
+      <c r="AT11">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU11">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47">
+      <c r="A12">
+        <v>0.8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12">
+        <v>4265</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1412</v>
+      </c>
+      <c r="E12">
+        <v>382.66838621531099</v>
+      </c>
+      <c r="G12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12">
+        <v>4265</v>
+      </c>
+      <c r="I12">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J12">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L12" t="s">
+        <v>136</v>
+      </c>
+      <c r="M12">
+        <v>4265</v>
+      </c>
+      <c r="N12">
+        <v>151.860726846424</v>
+      </c>
+      <c r="O12">
+        <v>32.397968254699997</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>140.91418522860451</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>136</v>
+      </c>
+      <c r="R12">
+        <v>4265</v>
+      </c>
+      <c r="S12">
+        <v>10.9465416178195</v>
+      </c>
+      <c r="T12">
+        <v>12.673928894139801</v>
+      </c>
+      <c r="V12" t="s">
+        <v>176</v>
+      </c>
+      <c r="W12">
+        <v>1366</v>
+      </c>
+      <c r="X12">
+        <v>174.442166910688</v>
+      </c>
+      <c r="Y12">
+        <v>31.250458530683701</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="1"/>
+        <v>46.784251107955498</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB12">
+        <v>1343</v>
+      </c>
+      <c r="AC12">
+        <v>187.69843633656001</v>
+      </c>
+      <c r="AD12">
+        <v>55.041488664945099</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN12">
+        <v>4265</v>
+      </c>
+      <c r="AO12">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP12">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AS12">
+        <v>4265</v>
+      </c>
+      <c r="AT12">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU12">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47">
+      <c r="A13">
+        <v>0.9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13">
+        <v>4265</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1410.59320046893</v>
+      </c>
+      <c r="E13">
+        <v>381.71928847997401</v>
+      </c>
+      <c r="G13" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13">
+        <v>4265</v>
+      </c>
+      <c r="I13">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J13">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L13" t="s">
+        <v>137</v>
+      </c>
+      <c r="M13">
+        <v>4265</v>
+      </c>
+      <c r="N13">
+        <v>124.602344665885</v>
+      </c>
+      <c r="O13">
+        <v>26.664449460758501</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>110.1652989449002</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>137</v>
+      </c>
+      <c r="R13">
+        <v>4265</v>
+      </c>
+      <c r="S13">
+        <v>14.4370457209848</v>
+      </c>
+      <c r="T13">
+        <v>11.954252883467699</v>
+      </c>
+      <c r="V13" t="s">
+        <v>178</v>
+      </c>
+      <c r="W13">
+        <v>1781</v>
+      </c>
+      <c r="X13">
+        <v>179.52161706906199</v>
+      </c>
+      <c r="Y13">
+        <v>31.911433069194601</v>
+      </c>
+      <c r="Z13">
+        <f>AC14-P13</f>
+        <v>-48.068678288070103</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB13">
+        <v>1744</v>
+      </c>
+      <c r="AC13">
+        <v>113.837155963303</v>
+      </c>
+      <c r="AD13">
+        <v>42.890939309686701</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN13">
+        <v>4265</v>
+      </c>
+      <c r="AO13">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP13">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS13">
+        <v>4265</v>
+      </c>
+      <c r="AT13">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU13">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47">
+      <c r="A14">
+        <v>0.95</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14">
+        <v>4265</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1405.7256740914399</v>
+      </c>
+      <c r="E14">
+        <v>360.79180532744499</v>
+      </c>
+      <c r="G14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14">
+        <v>4265</v>
+      </c>
+      <c r="I14">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J14">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L14" t="s">
+        <v>139</v>
+      </c>
+      <c r="M14">
+        <v>4265</v>
+      </c>
+      <c r="N14">
+        <v>82.684173505275496</v>
+      </c>
+      <c r="O14">
+        <v>20.602359548738999</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>63.656037514654194</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R14">
+        <v>4265</v>
+      </c>
+      <c r="S14">
+        <v>19.028135990621301</v>
+      </c>
+      <c r="T14">
+        <v>11.3704529670408</v>
+      </c>
+      <c r="V14" t="s">
+        <v>177</v>
+      </c>
+      <c r="W14">
+        <v>2148</v>
+      </c>
+      <c r="X14">
+        <v>189.471601489758</v>
+      </c>
+      <c r="Y14">
+        <v>31.264555195833601</v>
+      </c>
+      <c r="Z14">
+        <f>AC13-P14</f>
+        <v>50.18111844864881</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB14">
+        <v>2101</v>
+      </c>
+      <c r="AC14">
+        <v>62.096620656830098</v>
+      </c>
+      <c r="AD14">
+        <v>34.917954080186703</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AN14">
+        <v>4265</v>
+      </c>
+      <c r="AO14">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP14">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS14">
+        <v>4265</v>
+      </c>
+      <c r="AT14">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU14">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47">
+      <c r="B15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15">
+        <v>4265</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1451.76553341149</v>
+      </c>
+      <c r="E15">
+        <v>370.12522776019199</v>
+      </c>
+      <c r="G15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15">
+        <v>4265</v>
+      </c>
+      <c r="I15">
+        <v>6018.8752637749103</v>
+      </c>
+      <c r="J15">
+        <v>714.08855262149905</v>
+      </c>
+      <c r="L15" t="s">
+        <v>138</v>
+      </c>
+      <c r="M15">
+        <v>4265</v>
+      </c>
+      <c r="N15">
+        <v>50.288862837045698</v>
+      </c>
+      <c r="O15">
+        <v>18.362197336857601</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>32.701289566236795</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>138</v>
+      </c>
+      <c r="R15">
+        <v>4265</v>
+      </c>
+      <c r="S15">
+        <v>17.5875732708089</v>
+      </c>
+      <c r="T15">
+        <v>12.8278720546367</v>
+      </c>
+      <c r="Z15" t="e">
+        <f>#REF!-P15</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN15">
+        <v>4265</v>
+      </c>
+      <c r="AO15">
+        <v>3579.70996483001</v>
+      </c>
+      <c r="AP15">
+        <v>305.00852425055399</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>138</v>
+      </c>
+      <c r="AS15">
+        <v>4265</v>
+      </c>
+      <c r="AT15">
+        <v>2439.1652989448999</v>
+      </c>
+      <c r="AU15">
+        <v>569.50334186381497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47">
+      <c r="Z16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="26:47">
+      <c r="Z17" s="3">
+        <f>P5/AC5</f>
+        <v>0.57416904312044814</v>
+      </c>
+    </row>
+    <row r="18" spans="26:47">
+      <c r="Z18" s="3">
+        <f t="shared" ref="Z18:Z24" si="2">P6/AC6</f>
+        <v>0.57765326031339237</v>
+      </c>
+    </row>
+    <row r="19" spans="26:47">
+      <c r="Z19" s="3">
+        <f t="shared" si="2"/>
+        <v>0.59830411767823288</v>
+      </c>
+    </row>
+    <row r="20" spans="26:47">
+      <c r="Z20" s="3">
+        <f t="shared" si="2"/>
+        <v>0.61718062475076052</v>
+      </c>
+    </row>
+    <row r="21" spans="26:47">
+      <c r="Z21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.6358726002427576</v>
+      </c>
+    </row>
+    <row r="22" spans="26:47">
+      <c r="Z22" s="3">
+        <f t="shared" si="2"/>
+        <v>0.66853670641325635</v>
+      </c>
+    </row>
+    <row r="23" spans="26:47">
+      <c r="Z23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.69937584408624887</v>
+      </c>
+    </row>
+    <row r="24" spans="26:47">
+      <c r="Z24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.75074778447239077</v>
+      </c>
+    </row>
+    <row r="25" spans="26:47">
+      <c r="Z25" s="3">
+        <f>P13/AC14</f>
+        <v>1.7740949149828327</v>
+      </c>
+    </row>
+    <row r="26" spans="26:47">
+      <c r="Z26" s="3">
+        <f>P14/AC13</f>
+        <v>0.55918506550861657</v>
+      </c>
+    </row>
+    <row r="27" spans="26:47">
+      <c r="Z27" s="3" t="e">
+        <f>P15/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="28" spans="26:47">
+      <c r="AM28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="26:47">
+      <c r="AM29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN29" s="1">
+        <v>1464</v>
+      </c>
+      <c r="AO29" s="1">
+        <v>3600.1045079999999</v>
+      </c>
+      <c r="AP29" s="1">
+        <v>322.67472500000002</v>
+      </c>
+      <c r="AR29" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS29">
+        <v>1491</v>
+      </c>
+      <c r="AT29">
+        <v>2453.6277665995999</v>
+      </c>
+      <c r="AU29">
+        <v>549.89631750632998</v>
+      </c>
+    </row>
+    <row r="30" spans="26:47">
+      <c r="AM30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN30" s="1">
+        <v>1470</v>
+      </c>
+      <c r="AO30" s="1">
+        <v>3599.3224489999998</v>
+      </c>
+      <c r="AP30" s="1">
+        <v>322.32970990000001</v>
+      </c>
+      <c r="AR30" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS30">
+        <v>1501</v>
+      </c>
+      <c r="AT30">
+        <v>2452.04596935376</v>
+      </c>
+      <c r="AU30">
+        <v>548.76528426891502</v>
+      </c>
+    </row>
+    <row r="31" spans="26:47">
+      <c r="AM31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AN31" s="1">
+        <v>1472</v>
+      </c>
+      <c r="AO31" s="1">
+        <v>3599.3091030000001</v>
+      </c>
+      <c r="AP31" s="1">
+        <v>322.23685649999999</v>
+      </c>
+      <c r="AR31" t="s">
+        <v>157</v>
+      </c>
+      <c r="AS31">
+        <v>1503</v>
+      </c>
+      <c r="AT31">
+        <v>2452.1357285429099</v>
+      </c>
+      <c r="AU31">
+        <v>548.409477429356</v>
+      </c>
+    </row>
+    <row r="32" spans="26:47">
+      <c r="AM32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AN32" s="1">
+        <v>1477</v>
+      </c>
+      <c r="AO32" s="1">
+        <v>3600.6194989999999</v>
+      </c>
+      <c r="AP32" s="1">
+        <v>322.84104689999998</v>
+      </c>
+      <c r="AR32" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS32">
+        <v>1509</v>
+      </c>
+      <c r="AT32">
+        <v>2452.40490390987</v>
+      </c>
+      <c r="AU32">
+        <v>547.34953820989801</v>
+      </c>
+    </row>
+    <row r="33" spans="39:47">
+      <c r="AM33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AN33" s="1">
+        <v>1473</v>
+      </c>
+      <c r="AO33" s="1">
+        <v>3599.5736590000001</v>
+      </c>
+      <c r="AP33" s="1">
+        <v>322.2873649</v>
+      </c>
+      <c r="AR33" t="s">
+        <v>159</v>
+      </c>
+      <c r="AS33">
+        <v>1504</v>
+      </c>
+      <c r="AT33">
+        <v>2452.1728723404299</v>
+      </c>
+      <c r="AU33">
+        <v>548.22890126214895</v>
+      </c>
+    </row>
+    <row r="34" spans="39:47">
+      <c r="AM34" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN34" s="1">
+        <v>1470</v>
+      </c>
+      <c r="AO34" s="1">
+        <v>3599.3224489999998</v>
+      </c>
+      <c r="AP34" s="1">
+        <v>322.32970990000001</v>
+      </c>
+      <c r="AR34" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS34">
+        <v>1499</v>
+      </c>
+      <c r="AT34">
+        <v>2451.9666444296199</v>
+      </c>
+      <c r="AU34">
+        <v>549.12259322000295</v>
+      </c>
+    </row>
+    <row r="35" spans="39:47">
+      <c r="AM35" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AN35" s="1">
+        <v>1492</v>
+      </c>
+      <c r="AO35" s="1">
+        <v>3602.152145</v>
+      </c>
+      <c r="AP35" s="1">
+        <v>322.4974459</v>
+      </c>
+      <c r="AR35" t="s">
+        <v>161</v>
+      </c>
+      <c r="AS35">
+        <v>1518</v>
+      </c>
+      <c r="AT35">
+        <v>2453.2694334650901</v>
+      </c>
+      <c r="AU35">
+        <v>545.89095305868602</v>
+      </c>
+    </row>
+    <row r="36" spans="39:47">
+      <c r="AM36" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AN36" s="1">
+        <v>1480</v>
+      </c>
+      <c r="AO36" s="1">
+        <v>3601.528378</v>
+      </c>
+      <c r="AP36" s="1">
+        <v>323.1530333</v>
+      </c>
+      <c r="AR36" t="s">
+        <v>162</v>
+      </c>
+      <c r="AS36">
+        <v>1511</v>
+      </c>
+      <c r="AT36">
+        <v>2452.5512905360702</v>
+      </c>
+      <c r="AU36">
+        <v>547.00189823452604</v>
+      </c>
+    </row>
+    <row r="37" spans="39:47">
+      <c r="AM37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN37" s="1">
+        <v>1471</v>
+      </c>
+      <c r="AO37" s="1">
+        <v>3599.4819849999999</v>
+      </c>
+      <c r="AP37" s="1">
+        <v>322.2781463</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>163</v>
+      </c>
+      <c r="AS37">
+        <v>1501</v>
+      </c>
+      <c r="AT37">
+        <v>2452.04596935376</v>
+      </c>
+      <c r="AU37">
+        <v>548.76528426891502</v>
+      </c>
+    </row>
+    <row r="38" spans="39:47">
+      <c r="AM38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN38" s="1">
+        <v>1492</v>
+      </c>
+      <c r="AO38" s="1">
+        <v>3602.152145</v>
+      </c>
+      <c r="AP38" s="1">
+        <v>322.4974459</v>
+      </c>
+      <c r="AR38" t="s">
+        <v>164</v>
+      </c>
+      <c r="AS38">
+        <v>1519</v>
+      </c>
+      <c r="AT38">
+        <v>2453.5523370638598</v>
+      </c>
+      <c r="AU38">
+        <v>545.82249499294005</v>
+      </c>
+    </row>
+    <row r="39" spans="39:47">
+      <c r="AM39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AN39" s="1">
+        <v>1492</v>
+      </c>
+      <c r="AO39" s="1">
+        <v>3602.152145</v>
+      </c>
+      <c r="AP39" s="1">
+        <v>322.4974459</v>
+      </c>
+      <c r="AR39" t="s">
+        <v>165</v>
+      </c>
+      <c r="AS39">
+        <v>1518</v>
+      </c>
+      <c r="AT39">
+        <v>2453.2694334650901</v>
+      </c>
+      <c r="AU39">
+        <v>545.89095305868602</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T71"/>
@@ -19887,8 +23022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AU39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+    <sheetView topLeftCell="Z3" workbookViewId="0">
+      <selection activeCell="AT5" sqref="AT5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20141,7 +23276,7 @@
         <v>16.769014026125799</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z15" si="1">AC6-P6</f>
+        <f t="shared" ref="Z6:Z14" si="1">AC6-P6</f>
         <v>146.30128956623668</v>
       </c>
       <c r="AA6" t="s">
@@ -20904,7 +24039,7 @@
         <v>10.6022729291426</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="1"/>
+        <f>AC13-P13</f>
         <v>96.570457209847802</v>
       </c>
       <c r="AA13" t="s">
@@ -21122,7 +24257,7 @@
         <v>4.4792909639774896</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="1"/>
+        <f>AC15-P15</f>
         <v>37.564126611957803</v>
       </c>
       <c r="AA15" t="s">
@@ -21223,13 +24358,13 @@
     </row>
     <row r="26" spans="26:47">
       <c r="Z26" s="3">
-        <f t="shared" ref="Z26:Z44" si="3">P14/AC14</f>
+        <f t="shared" ref="Z26" si="3">P14/AC14</f>
         <v>0.49780428727807019</v>
       </c>
     </row>
     <row r="27" spans="26:47">
       <c r="Z27" s="3">
-        <f t="shared" si="3"/>
+        <f>P15/AC15</f>
         <v>0.4653966537863467</v>
       </c>
     </row>

</xml_diff>

<commit_message>
the first full version of the paper
</commit_message>
<xml_diff>
--- a/write-ups/cikm/performance.xlsx
+++ b/write-ups/cikm/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Change with Epochlength" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="jaccard+May5th" sheetId="9" r:id="rId9"/>
     <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
     <sheet name="jaccard+May5th (2)" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="181">
   <si>
     <t>MinSupp</t>
   </si>
@@ -572,6 +573,12 @@
   <si>
     <t>LCM + Clustering</t>
   </si>
+  <si>
+    <t>Frequent items</t>
+  </si>
+  <si>
+    <t>Len2+ Max</t>
+  </si>
 </sst>
 </file>
 
@@ -632,8 +639,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="327">
+  <cellStyleXfs count="347">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -970,7 +997,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="327">
+  <cellStyles count="347">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1134,6 +1161,16 @@
     <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1297,6 +1334,16 @@
     <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1486,11 +1533,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130156344"/>
-        <c:axId val="-2130162360"/>
+        <c:axId val="-2062670744"/>
+        <c:axId val="-2062667752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130156344"/>
+        <c:axId val="-2062670744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,7 +1547,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130162360"/>
+        <c:crossAx val="-2062667752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1508,7 +1555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130162360"/>
+        <c:axId val="-2062667752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1519,7 +1566,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130156344"/>
+        <c:crossAx val="-2062670744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1626,11 +1673,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="2126422216"/>
-        <c:axId val="2126420440"/>
+        <c:axId val="-2060742392"/>
+        <c:axId val="2084935032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126422216"/>
+        <c:axId val="-2060742392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1639,7 +1686,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126420440"/>
+        <c:crossAx val="2084935032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1647,7 +1694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126420440"/>
+        <c:axId val="2084935032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1704,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126422216"/>
+        <c:crossAx val="-2060742392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1745,11 +1792,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="2126459032"/>
-        <c:axId val="2126462008"/>
+        <c:axId val="-2063435560"/>
+        <c:axId val="-2063536360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126459032"/>
+        <c:axId val="-2063435560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1758,7 +1805,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126462008"/>
+        <c:crossAx val="-2063536360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1766,7 +1813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126462008"/>
+        <c:axId val="-2063536360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1776,7 +1823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126459032"/>
+        <c:crossAx val="-2063435560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2018,11 +2065,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2126493992"/>
-        <c:axId val="-2126490904"/>
+        <c:axId val="-2062990744"/>
+        <c:axId val="-2062987768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2126493992"/>
+        <c:axId val="-2062990744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2032,7 +2079,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126490904"/>
+        <c:crossAx val="-2062987768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2040,7 +2087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126490904"/>
+        <c:axId val="-2062987768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2051,7 +2098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126493992"/>
+        <c:crossAx val="-2062990744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2168,11 +2215,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="-2113928040"/>
-        <c:axId val="-2113062056"/>
+        <c:axId val="-2063523528"/>
+        <c:axId val="-2062811304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113928040"/>
+        <c:axId val="-2063523528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2182,7 +2229,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113062056"/>
+        <c:crossAx val="-2062811304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2190,7 +2237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113062056"/>
+        <c:axId val="-2062811304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2247,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113928040"/>
+        <c:crossAx val="-2063523528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2369,11 +2416,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Extension!$D$12</c:f>
+              <c:f>Extension!$E$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Maximal Itemsets</c:v>
+                  <c:v>Len2+ Max</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2404,24 +2451,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Extension!$D$13:$D$17</c:f>
+              <c:f>Extension!$E$13:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10193.3824</c:v>
+                  <c:v>4541.1242</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5539.2927</c:v>
+                  <c:v>1831.9194</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5303.5682</c:v>
+                  <c:v>1757.9123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5287.3667</c:v>
+                  <c:v>1736.339499999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5153.8462</c:v>
+                  <c:v>1683.5129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2436,11 +2483,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2125893096"/>
-        <c:axId val="2125890104"/>
+        <c:axId val="-2083268664"/>
+        <c:axId val="-2083265688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125893096"/>
+        <c:axId val="-2083268664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,7 +2496,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125890104"/>
+        <c:crossAx val="-2083265688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2457,7 +2504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125890104"/>
+        <c:axId val="-2083265688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2468,7 +2515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125893096"/>
+        <c:crossAx val="-2083268664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2752,11 +2799,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2125852264"/>
-        <c:axId val="2125849128"/>
+        <c:axId val="-2082588504"/>
+        <c:axId val="-2083187864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125852264"/>
+        <c:axId val="-2082588504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2765,7 +2812,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125849128"/>
+        <c:crossAx val="-2083187864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2773,7 +2820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125849128"/>
+        <c:axId val="-2083187864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2788,7 +2835,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125852264"/>
+        <c:crossAx val="-2082588504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2926,11 +2973,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125820088"/>
-        <c:axId val="2125817128"/>
+        <c:axId val="-2123573928"/>
+        <c:axId val="2084647944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125820088"/>
+        <c:axId val="-2123573928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2939,7 +2986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125817128"/>
+        <c:crossAx val="2084647944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2947,7 +2994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125817128"/>
+        <c:axId val="2084647944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2958,7 +3005,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125820088"/>
+        <c:crossAx val="-2123573928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3057,11 +3104,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125791832"/>
-        <c:axId val="2125788872"/>
+        <c:axId val="-2060966792"/>
+        <c:axId val="-2061062824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125791832"/>
+        <c:axId val="-2060966792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3070,7 +3117,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125788872"/>
+        <c:crossAx val="-2061062824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3078,7 +3125,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125788872"/>
+        <c:axId val="-2061062824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3089,7 +3136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125791832"/>
+        <c:crossAx val="-2060966792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3178,11 +3225,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125752008"/>
-        <c:axId val="2125749048"/>
+        <c:axId val="-2063337080"/>
+        <c:axId val="-2063334136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125752008"/>
+        <c:axId val="-2063337080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3191,7 +3238,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125749048"/>
+        <c:crossAx val="-2063334136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3199,7 +3246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125749048"/>
+        <c:axId val="-2063334136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3210,7 +3257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125752008"/>
+        <c:crossAx val="-2063337080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3299,11 +3346,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125722408"/>
-        <c:axId val="2125719448"/>
+        <c:axId val="-2063365816"/>
+        <c:axId val="-2063570888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125722408"/>
+        <c:axId val="-2063365816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3312,7 +3359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125719448"/>
+        <c:crossAx val="-2063570888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3320,7 +3367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125719448"/>
+        <c:axId val="-2063570888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3331,7 +3378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125722408"/>
+        <c:crossAx val="-2063365816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3433,11 +3480,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130089992"/>
-        <c:axId val="-2130086984"/>
+        <c:axId val="-2063511176"/>
+        <c:axId val="-2062651800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130089992"/>
+        <c:axId val="-2063511176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3446,7 +3493,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130086984"/>
+        <c:crossAx val="-2062651800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3454,7 +3501,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130086984"/>
+        <c:axId val="-2062651800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3469,7 +3516,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130089992"/>
+        <c:crossAx val="-2063511176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3584,11 +3631,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2125690008"/>
-        <c:axId val="2125687016"/>
+        <c:axId val="-2061032440"/>
+        <c:axId val="-2124230536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125690008"/>
+        <c:axId val="-2061032440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3597,7 +3644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125687016"/>
+        <c:crossAx val="-2124230536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3605,7 +3652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125687016"/>
+        <c:axId val="-2124230536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3616,7 +3663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125690008"/>
+        <c:crossAx val="-2061032440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3730,11 +3777,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2125659912"/>
-        <c:axId val="2125656920"/>
+        <c:axId val="-2084079768"/>
+        <c:axId val="-2084564968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125659912"/>
+        <c:axId val="-2084079768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3743,7 +3790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125656920"/>
+        <c:crossAx val="-2084564968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3751,7 +3798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125656920"/>
+        <c:axId val="-2084564968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3762,7 +3809,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125659912"/>
+        <c:crossAx val="-2084079768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3901,11 +3948,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125618712"/>
-        <c:axId val="2125613368"/>
+        <c:axId val="-2083924392"/>
+        <c:axId val="-2083904072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125618712"/>
+        <c:axId val="-2083924392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3934,7 +3981,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125613368"/>
+        <c:crossAx val="-2083904072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3942,7 +3989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125613368"/>
+        <c:axId val="-2083904072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3953,7 +4000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125618712"/>
+        <c:crossAx val="-2083924392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4052,11 +4099,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2129825528"/>
-        <c:axId val="-2129822520"/>
+        <c:axId val="-2083400072"/>
+        <c:axId val="2084653496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129825528"/>
+        <c:axId val="-2083400072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4065,7 +4112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129822520"/>
+        <c:crossAx val="2084653496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4073,7 +4120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129822520"/>
+        <c:axId val="2084653496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4084,7 +4131,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129825528"/>
+        <c:crossAx val="-2083400072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4201,11 +4248,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2119106104"/>
-        <c:axId val="-2118888488"/>
+        <c:axId val="-2062058712"/>
+        <c:axId val="-2062055704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2119106104"/>
+        <c:axId val="-2062058712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4214,7 +4261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118888488"/>
+        <c:crossAx val="-2062055704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4222,7 +4269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2118888488"/>
+        <c:axId val="-2062055704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4233,7 +4280,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119106104"/>
+        <c:crossAx val="-2062058712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4440,7 +4487,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4450,11 +4496,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2119027320"/>
-        <c:axId val="-2093449176"/>
+        <c:axId val="-2062024136"/>
+        <c:axId val="-2062021160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2119027320"/>
+        <c:axId val="-2062024136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4464,7 +4510,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093449176"/>
+        <c:crossAx val="-2062021160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4472,7 +4518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093449176"/>
+        <c:axId val="-2062021160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4482,7 +4528,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119027320"/>
+        <c:crossAx val="-2062024136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4634,11 +4680,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2107929432"/>
-        <c:axId val="-2107854392"/>
+        <c:axId val="-2061995544"/>
+        <c:axId val="-2061992568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2107929432"/>
+        <c:axId val="-2061995544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4647,7 +4693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107854392"/>
+        <c:crossAx val="-2061992568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4655,7 +4701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107854392"/>
+        <c:axId val="-2061992568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4666,7 +4712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107929432"/>
+        <c:crossAx val="-2061995544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4822,11 +4868,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2118905112"/>
-        <c:axId val="-2093942920"/>
+        <c:axId val="-2061967176"/>
+        <c:axId val="-2061962024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2118905112"/>
+        <c:axId val="-2061967176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4840,7 +4886,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093942920"/>
+        <c:crossAx val="-2061962024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4848,7 +4894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093942920"/>
+        <c:axId val="-2061962024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4863,7 +4909,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118905112"/>
+        <c:crossAx val="-2061967176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4900,7 +4946,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4977,11 +5022,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2095902568"/>
-        <c:axId val="-2108644776"/>
+        <c:axId val="-2061936200"/>
+        <c:axId val="-2061933192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095902568"/>
+        <c:axId val="-2061936200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4990,7 +5035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108644776"/>
+        <c:crossAx val="-2061933192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4998,7 +5043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108644776"/>
+        <c:axId val="-2061933192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5009,14 +5054,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2095902568"/>
+        <c:crossAx val="-2061936200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5273,11 +5317,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="-2093344584"/>
-        <c:axId val="-2090212792"/>
+        <c:axId val="-2061894888"/>
+        <c:axId val="-2061891768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2093344584"/>
+        <c:axId val="-2061894888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,7 +5331,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090212792"/>
+        <c:crossAx val="-2061891768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5295,7 +5339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090212792"/>
+        <c:axId val="-2061891768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5306,7 +5350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093344584"/>
+        <c:crossAx val="-2061894888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5317,7 +5361,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5678,11 +5721,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2130049752"/>
-        <c:axId val="-2130044360"/>
+        <c:axId val="2086242520"/>
+        <c:axId val="-2062682856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2130049752"/>
+        <c:axId val="2086242520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5711,7 +5754,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130044360"/>
+        <c:crossAx val="-2062682856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5719,7 +5762,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130044360"/>
+        <c:axId val="-2062682856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5729,7 +5772,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130049752"/>
+        <c:crossAx val="2086242520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5774,7 +5817,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5851,11 +5893,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2092712536"/>
-        <c:axId val="-2092709528"/>
+        <c:axId val="-2061872760"/>
+        <c:axId val="-2061869768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2092712536"/>
+        <c:axId val="-2061872760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5864,7 +5906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092709528"/>
+        <c:crossAx val="-2061869768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5872,7 +5914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2092709528"/>
+        <c:axId val="-2061869768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5883,14 +5925,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092712536"/>
+        <c:crossAx val="-2061872760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6090,11 +6131,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2091628136"/>
-        <c:axId val="-2090930696"/>
+        <c:axId val="-2061835448"/>
+        <c:axId val="-2061832472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2091628136"/>
+        <c:axId val="-2061835448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6104,7 +6145,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090930696"/>
+        <c:crossAx val="-2061832472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6112,7 +6153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090930696"/>
+        <c:axId val="-2061832472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6122,7 +6163,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091628136"/>
+        <c:crossAx val="-2061835448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6268,11 +6309,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123898904"/>
-        <c:axId val="-2084655608"/>
+        <c:axId val="-2061806824"/>
+        <c:axId val="-2061803848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123898904"/>
+        <c:axId val="-2061806824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6281,7 +6322,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2084655608"/>
+        <c:crossAx val="-2061803848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6289,7 +6330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2084655608"/>
+        <c:axId val="-2061803848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6300,7 +6341,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123898904"/>
+        <c:crossAx val="-2061806824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6450,11 +6491,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2094592184"/>
-        <c:axId val="-2093289064"/>
+        <c:axId val="-2061778456"/>
+        <c:axId val="-2061773304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2094592184"/>
+        <c:axId val="-2061778456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6468,7 +6509,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093289064"/>
+        <c:crossAx val="-2061773304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6476,7 +6517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093289064"/>
+        <c:axId val="-2061773304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6491,7 +6532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094592184"/>
+        <c:crossAx val="-2061778456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6602,11 +6643,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2088149304"/>
-        <c:axId val="-2088415816"/>
+        <c:axId val="-2061748632"/>
+        <c:axId val="-2061745688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2088149304"/>
+        <c:axId val="-2061748632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6615,7 +6656,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088415816"/>
+        <c:crossAx val="-2061745688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6623,7 +6664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2088415816"/>
+        <c:axId val="-2061745688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6634,7 +6675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088149304"/>
+        <c:crossAx val="-2061748632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6889,11 +6930,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="-2087918456"/>
-        <c:axId val="-2093466712"/>
+        <c:axId val="-2061707112"/>
+        <c:axId val="-2061703992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2087918456"/>
+        <c:axId val="-2061707112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6903,7 +6944,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093466712"/>
+        <c:crossAx val="-2061703992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6911,7 +6952,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093466712"/>
+        <c:axId val="-2061703992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6922,7 +6963,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087918456"/>
+        <c:crossAx val="-2061707112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7042,11 +7083,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2130023640"/>
-        <c:axId val="-2130020632"/>
+        <c:axId val="-2063123528"/>
+        <c:axId val="-2063120472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130023640"/>
+        <c:axId val="-2063123528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7055,7 +7096,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130020632"/>
+        <c:crossAx val="-2063120472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7063,7 +7104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130020632"/>
+        <c:axId val="-2063120472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7078,7 +7119,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130023640"/>
+        <c:crossAx val="-2063123528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7247,11 +7288,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="-2129985096"/>
-        <c:axId val="-2129982120"/>
+        <c:axId val="-2063456024"/>
+        <c:axId val="-2063453048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129985096"/>
+        <c:axId val="-2063456024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7260,7 +7301,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129982120"/>
+        <c:crossAx val="-2063453048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7268,7 +7309,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129982120"/>
+        <c:axId val="-2063453048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7298,7 +7339,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129985096"/>
+        <c:crossAx val="-2063456024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7435,11 +7476,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2129950392"/>
-        <c:axId val="-2129947416"/>
+        <c:axId val="-2062860376"/>
+        <c:axId val="-2062857400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129950392"/>
+        <c:axId val="-2062860376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7448,7 +7489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129947416"/>
+        <c:crossAx val="-2062857400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7456,7 +7497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129947416"/>
+        <c:axId val="-2062857400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7467,7 +7508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129950392"/>
+        <c:crossAx val="-2062860376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7729,11 +7770,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2129914968"/>
-        <c:axId val="-2129911992"/>
+        <c:axId val="-2063236456"/>
+        <c:axId val="-2062941480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2129914968"/>
+        <c:axId val="-2063236456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7742,7 +7783,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129911992"/>
+        <c:crossAx val="-2062941480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7750,7 +7791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129911992"/>
+        <c:axId val="-2062941480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7761,7 +7802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129914968"/>
+        <c:crossAx val="-2063236456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8014,11 +8055,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2129876376"/>
-        <c:axId val="-2129873400"/>
+        <c:axId val="-2062836760"/>
+        <c:axId val="-2062833784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2129876376"/>
+        <c:axId val="-2062836760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8027,7 +8068,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129873400"/>
+        <c:crossAx val="-2062833784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8035,7 +8076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129873400"/>
+        <c:axId val="-2062833784"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -8054,7 +8095,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Log of time in milliseconds</a:t>
+                  <a:t>Time in milliseconds</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8063,7 +8104,7 @@
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -8073,12 +8114,9 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2129876376"/>
+        <c:crossAx val="-2062836760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="thousands"/>
-        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -8268,11 +8306,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="-2126354088"/>
-        <c:axId val="-2115596488"/>
+        <c:axId val="2112421672"/>
+        <c:axId val="2127696168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2126354088"/>
+        <c:axId val="2112421672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8281,7 +8319,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115596488"/>
+        <c:crossAx val="2127696168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8289,7 +8327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115596488"/>
+        <c:axId val="2127696168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8305,7 +8343,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2126354088"/>
+        <c:crossAx val="2112421672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9768,8 +9806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S976"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16533,7 +16571,7 @@
         <v>31.1157426881209</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6:P15" si="0">N6-S6</f>
+        <f t="shared" ref="P6:P14" si="0">N6-S6</f>
         <v>170.22128060263699</v>
       </c>
       <c r="Q6" t="s">
@@ -16561,7 +16599,7 @@
         <v>31.174880247541001</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z15" si="1">AC6-P6</f>
+        <f t="shared" ref="Z6:Z14" si="1">AC6-P6</f>
         <v>188.18727970864703</v>
       </c>
       <c r="AA6" t="s">
@@ -17877,6 +17915,23 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -19048,8 +19103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19636,6 +19691,12 @@
       <c r="D12" t="s">
         <v>125</v>
       </c>
+      <c r="E12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G12" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="13" spans="1:35">
       <c r="B13" t="s">
@@ -19644,6 +19705,14 @@
       <c r="D13">
         <v>10193.3824</v>
       </c>
+      <c r="E13">
+        <f>D13-G13</f>
+        <v>4541.1242000000011</v>
+      </c>
+      <c r="G13">
+        <f>D4-K4</f>
+        <v>5652.2581999999993</v>
+      </c>
     </row>
     <row r="14" spans="1:35">
       <c r="B14" t="s">
@@ -19652,6 +19721,14 @@
       <c r="D14">
         <v>5539.2927</v>
       </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E17" si="0">D14-G14</f>
+        <v>1831.9194000000002</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G17" si="1">D5-K5</f>
+        <v>3707.3732999999997</v>
+      </c>
     </row>
     <row r="15" spans="1:35">
       <c r="B15" t="s">
@@ -19660,6 +19737,14 @@
       <c r="D15">
         <v>5303.5681999999997</v>
       </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1757.9122999999995</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>3545.6559000000002</v>
+      </c>
     </row>
     <row r="16" spans="1:35">
       <c r="B16" t="s">
@@ -19668,6 +19753,14 @@
       <c r="D16">
         <v>5287.3666999999996</v>
       </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1736.3394999999991</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>3551.0272000000004</v>
+      </c>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" t="s">
@@ -19675,6 +19768,14 @@
       </c>
       <c r="D17">
         <v>5153.8462</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1683.5128999999997</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>3470.3333000000002</v>
       </c>
     </row>
     <row r="30" spans="2:9">
@@ -19877,7 +19978,7 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="AA38" sqref="AA38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20075,7 +20176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:P12"/>
     </sheetView>
   </sheetViews>
@@ -22147,8 +22248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>